<commit_message>
Update Forms to use repeat_count
</commit_message>
<xml_diff>
--- a/app/src/main/res/raw/change_head_form.xlsx
+++ b/app/src/main/res/raw/change_head_form.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="29550" windowHeight="11970" tabRatio="500"/>
+    <workbookView windowWidth="26265" windowHeight="9390" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="columns" sheetId="1" r:id="rId1"/>
@@ -70,7 +70,7 @@
     <t>options</t>
   </si>
   <si>
-    <t>foreach_count</t>
+    <t>repeat_count</t>
   </si>
   <si>
     <t>label</t>
@@ -199,7 +199,7 @@
     <t>relationships</t>
   </si>
   <si>
-    <t>start foreach</t>
+    <t>start repeat</t>
   </si>
   <si>
     <t xml:space="preserve">$household_residents </t>
@@ -241,7 +241,7 @@
     <t>5.3. Relação com o novo chefe do agregado</t>
   </si>
   <si>
-    <t>end foreach</t>
+    <t>end repeat</t>
   </si>
   <si>
     <t>collected</t>
@@ -501,9 +501,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="29">
@@ -549,10 +549,25 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -564,6 +579,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -573,7 +595,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F76"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -587,8 +609,62 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -602,88 +678,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -692,9 +686,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF9C6500"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -732,187 +732,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -926,26 +926,26 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -976,26 +976,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1023,151 +1014,160 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1556,8 +1556,8 @@
   <sheetPr/>
   <dimension ref="A1:O33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="12.75"/>

</xml_diff>

<commit_message>
Add Change Head of Household Form feature to HDS-Explorer
</commit_message>
<xml_diff>
--- a/app/src/main/res/raw/change_head_form.xlsx
+++ b/app/src/main/res/raw/change_head_form.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="26265" windowHeight="9390" tabRatio="500"/>
+    <workbookView windowWidth="28650" windowHeight="11985" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="columns" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="154">
   <si>
     <t>group</t>
   </si>
@@ -139,6 +139,9 @@
     <t>2.2. Nome do antigo chefe do agregado</t>
   </si>
   <si>
+    <t>newhead</t>
+  </si>
+  <si>
     <t>newHeadCode</t>
   </si>
   <si>
@@ -211,6 +214,9 @@
     <t>5. Relação dos membros com o novo chefe do agregado</t>
   </si>
   <si>
+    <t>newheadrelat</t>
+  </si>
+  <si>
     <t>newMemberCode</t>
   </si>
   <si>
@@ -487,6 +493,15 @@
     <t>form_name::pt</t>
   </si>
   <si>
+    <t>form_version</t>
+  </si>
+  <si>
+    <t>repeat_name</t>
+  </si>
+  <si>
+    <t>xml_node_name</t>
+  </si>
+  <si>
     <t>rawChangeHead</t>
   </si>
   <si>
@@ -494,6 +509,9 @@
   </si>
   <si>
     <t>Mudança do chefe do agregado</t>
+  </si>
+  <si>
+    <t>rawChangeHeadRelationship</t>
   </si>
 </sst>
 </file>
@@ -501,10 +519,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="29">
     <font>
@@ -547,6 +565,36 @@
       <color theme="0"/>
       <name val="Arial"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <u/>
@@ -558,14 +606,105 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Arial"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -579,127 +718,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="9"/>
       <name val="Times New Roman"/>
       <charset val="0"/>
@@ -732,31 +750,109 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -768,19 +864,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -792,127 +906,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -926,17 +944,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -965,6 +983,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -972,21 +1005,6 @@
       </top>
       <bottom style="double">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1026,148 +1044,148 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="25" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1557,7 +1575,7 @@
   <dimension ref="A1:O33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="A6" sqref="A6:H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="12.75"/>
@@ -1653,7 +1671,9 @@
       <c r="N2" s="17"/>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" s="1"/>
+      <c r="A3" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="18" t="s">
@@ -1732,19 +1752,21 @@
       </c>
     </row>
     <row r="6" spans="1:13">
-      <c r="A6" s="1"/>
+      <c r="A6" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="D6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E6" t="s">
         <v>17</v>
       </c>
       <c r="G6" s="24"/>
       <c r="H6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="J6" s="28"/>
       <c r="K6" s="28"/>
@@ -1756,19 +1778,21 @@
       </c>
     </row>
     <row r="7" spans="1:13">
-      <c r="A7" s="1"/>
+      <c r="A7" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="D7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E7" t="s">
         <v>17</v>
       </c>
       <c r="G7" s="24"/>
       <c r="H7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J7" s="28"/>
       <c r="K7" s="28"/>
@@ -1782,17 +1806,17 @@
     <row r="8" ht="13" customHeight="1" spans="1:12">
       <c r="A8" s="1"/>
       <c r="D8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E8" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G8" s="24"/>
       <c r="H8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J8" s="28"/>
       <c r="K8" s="28"/>
@@ -1803,20 +1827,20 @@
     <row r="9" spans="1:12">
       <c r="A9" s="1"/>
       <c r="D9" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F9" s="24" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G9" s="24"/>
       <c r="H9" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J9" s="28"/>
       <c r="K9" s="28"/>
@@ -1827,17 +1851,17 @@
     <row r="10" spans="1:14">
       <c r="A10" s="1"/>
       <c r="D10" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E10" t="s">
         <v>17</v>
       </c>
       <c r="G10" s="24"/>
       <c r="H10" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J10" s="28"/>
       <c r="K10" s="28"/>
@@ -1845,7 +1869,7 @@
         <v>1</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:15">
@@ -1853,20 +1877,20 @@
       <c r="B11" s="20"/>
       <c r="C11" s="20"/>
       <c r="D11" s="21" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E11" s="21" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F11" s="25"/>
       <c r="G11" s="25" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H11" s="26" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="I11" s="26" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="J11" s="29"/>
       <c r="K11" s="29"/>
@@ -1878,20 +1902,22 @@
       <c r="O11" s="26"/>
     </row>
     <row r="12" spans="1:13">
-      <c r="A12" s="22"/>
+      <c r="A12" s="22" t="s">
+        <v>54</v>
+      </c>
       <c r="B12" s="23"/>
       <c r="C12" s="23"/>
       <c r="D12" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E12" t="s">
         <v>17</v>
       </c>
       <c r="H12" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="I12" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="J12" s="28"/>
       <c r="K12" s="28"/>
@@ -1903,20 +1929,22 @@
       </c>
     </row>
     <row r="13" spans="1:13">
-      <c r="A13" s="22"/>
+      <c r="A13" s="22" t="s">
+        <v>54</v>
+      </c>
       <c r="B13" s="23"/>
       <c r="C13" s="23"/>
       <c r="D13" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E13" t="s">
         <v>17</v>
       </c>
       <c r="H13" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="I13" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="J13" s="28"/>
       <c r="K13" s="28"/>
@@ -1932,19 +1960,19 @@
       <c r="B14" s="23"/>
       <c r="C14" s="23"/>
       <c r="D14" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E14" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="F14" s="17" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H14" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="I14" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="J14" s="28"/>
       <c r="K14" s="28"/>
@@ -1957,10 +1985,10 @@
       <c r="B15" s="20"/>
       <c r="C15" s="20"/>
       <c r="D15" s="21" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E15" s="21" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F15" s="27"/>
       <c r="G15" s="27"/>
@@ -1975,19 +2003,19 @@
     </row>
     <row r="16" spans="1:13">
       <c r="A16" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D16" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E16" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H16" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="I16" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="J16" s="28"/>
       <c r="K16" s="28"/>
@@ -2000,19 +2028,19 @@
     </row>
     <row r="17" spans="1:13">
       <c r="A17" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D17" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E17" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="H17" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="I17" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="J17" s="28"/>
       <c r="K17" s="28"/>
@@ -2025,19 +2053,19 @@
     </row>
     <row r="18" spans="1:13">
       <c r="A18" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D18" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E18" t="s">
         <v>17</v>
       </c>
       <c r="H18" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="I18" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="J18" s="28"/>
       <c r="K18" s="28"/>
@@ -2131,7 +2159,7 @@
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C1" t="s">
         <v>7</v>
@@ -2145,303 +2173,303 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B2" s="1" t="b">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B3" s="1" t="b">
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E4" s="3"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="E5" s="3"/>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C15" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="D15" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="16" s="2" customFormat="1" spans="1:4">
       <c r="A16" s="8" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="17" s="2" customFormat="1" spans="1:4">
       <c r="A17" s="8" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="18" s="2" customFormat="1" spans="1:4">
       <c r="A18" s="8" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="19" s="2" customFormat="1" spans="1:4">
       <c r="A19" s="8" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row r="20" s="2" customFormat="1" spans="1:4">
       <c r="A20" s="8" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="21" s="2" customFormat="1" spans="1:4">
       <c r="A21" s="8" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="22" s="2" customFormat="1" spans="1:4">
       <c r="A22" s="8" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -2580,39 +2608,60 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelRow="1" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelRow="1" outlineLevelCol="5"/>
   <cols>
     <col min="1" max="1" width="21.7142857142857" customWidth="1"/>
     <col min="2" max="2" width="28.2857142857143" customWidth="1"/>
     <col min="3" max="3" width="29.7142857142857" customWidth="1"/>
+    <col min="4" max="4" width="12.5714285714286" customWidth="1"/>
+    <col min="5" max="5" width="16.7142857142857" customWidth="1"/>
+    <col min="6" max="6" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="C1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>146</v>
+      </c>
+      <c r="D1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="B2" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="C2" t="s">
-        <v>147</v>
+        <v>152</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>153</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add support for more collected Id's variables to enable better double id verification
</commit_message>
<xml_diff>
--- a/app/src/main/res/raw/change_head_form.xlsx
+++ b/app/src/main/res/raw/change_head_form.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="13605" tabRatio="500"/>
+    <workbookView xWindow="18420" yWindow="5850" windowWidth="9210" windowHeight="6465" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="columns" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="203">
   <si>
     <t>group</t>
   </si>
@@ -100,6 +100,9 @@
     <t>display_style</t>
   </si>
   <si>
+    <t>hidden</t>
+  </si>
+  <si>
     <t>header</t>
   </si>
   <si>
@@ -326,6 +329,27 @@
   </si>
   <si>
     <t>6.2. Date de la visite</t>
+  </si>
+  <si>
+    <t>collectedDeviceId</t>
+  </si>
+  <si>
+    <t>device_id</t>
+  </si>
+  <si>
+    <t>Device Id</t>
+  </si>
+  <si>
+    <t>collectedHouseholdId</t>
+  </si>
+  <si>
+    <t>Collected Household Id</t>
+  </si>
+  <si>
+    <t>collectedMemberId</t>
+  </si>
+  <si>
+    <t>Collected Member Id</t>
   </si>
   <si>
     <t>modules</t>
@@ -642,10 +666,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -700,14 +724,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Arial"/>
@@ -716,62 +732,15 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Arial"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -792,31 +761,32 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF800080"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF006100"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Arial"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -829,8 +799,62 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -874,43 +898,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -922,139 +1066,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1092,11 +1116,26 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1117,16 +1156,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1157,168 +1196,153 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1328,7 +1352,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1389,6 +1413,10 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1398,6 +1426,10 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1712,10 +1744,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:P33"/>
+  <dimension ref="A1:Q36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
+      <selection activeCell="M18" sqref="M18:M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="12.75"/>
@@ -1735,7 +1767,7 @@
     <col min="16" max="16" width="13.4571428571429" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:17">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1781,30 +1813,33 @@
       <c r="O1" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="34" t="s">
         <v>15</v>
+      </c>
+      <c r="Q1" s="34" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:15">
       <c r="A2" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="22" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E2" s="22" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H2" s="22" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
@@ -1818,24 +1853,24 @@
     </row>
     <row r="3" spans="1:15">
       <c r="A3" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="22" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E3" s="22" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H3" s="22" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
@@ -1849,25 +1884,25 @@
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="K4" s="29"/>
-      <c r="L4" s="29"/>
+        <v>31</v>
+      </c>
+      <c r="K4" s="31"/>
+      <c r="L4" s="31"/>
       <c r="M4" t="b">
         <v>1</v>
       </c>
@@ -1877,25 +1912,25 @@
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="K5" s="29"/>
-      <c r="L5" s="29"/>
+        <v>35</v>
+      </c>
+      <c r="K5" s="31"/>
+      <c r="L5" s="31"/>
       <c r="M5" t="b">
         <v>1</v>
       </c>
@@ -1905,25 +1940,25 @@
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="K6" s="29"/>
-      <c r="L6" s="29"/>
+        <v>40</v>
+      </c>
+      <c r="K6" s="31"/>
+      <c r="L6" s="31"/>
       <c r="M6" t="b">
         <v>1</v>
       </c>
@@ -1933,25 +1968,25 @@
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="K7" s="29"/>
-      <c r="L7" s="29"/>
+        <v>44</v>
+      </c>
+      <c r="K7" s="31"/>
+      <c r="L7" s="31"/>
       <c r="M7" t="b">
         <v>1</v>
       </c>
@@ -1962,22 +1997,22 @@
     <row r="8" ht="13" customHeight="1" spans="1:13">
       <c r="A8" s="1"/>
       <c r="D8" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E8" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H8" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I8" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="K8" s="29"/>
-      <c r="L8" s="29"/>
+        <v>49</v>
+      </c>
+      <c r="K8" s="31"/>
+      <c r="L8" s="31"/>
       <c r="M8" t="b">
         <v>1</v>
       </c>
@@ -1985,25 +2020,25 @@
     <row r="9" spans="1:13">
       <c r="A9" s="1"/>
       <c r="D9" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F9" s="21" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H9" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="I9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="K9" s="29"/>
-      <c r="L9" s="29"/>
+        <v>55</v>
+      </c>
+      <c r="K9" s="31"/>
+      <c r="L9" s="31"/>
       <c r="M9" t="b">
         <v>1</v>
       </c>
@@ -2011,27 +2046,27 @@
     <row r="10" spans="1:15">
       <c r="A10" s="1"/>
       <c r="D10" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H10" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I10" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="K10" s="29"/>
-      <c r="L10" s="29"/>
+        <v>59</v>
+      </c>
+      <c r="K10" s="31"/>
+      <c r="L10" s="31"/>
       <c r="M10" t="b">
         <v>1</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:16">
@@ -2039,54 +2074,54 @@
       <c r="B11" s="24"/>
       <c r="C11" s="24"/>
       <c r="D11" s="25" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E11" s="25" t="s">
-        <v>61</v>
-      </c>
-      <c r="F11" s="26"/>
-      <c r="G11" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="H11" s="27" t="s">
+      <c r="F11" s="28"/>
+      <c r="G11" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="I11" s="27" t="s">
+      <c r="H11" s="29" t="s">
         <v>64</v>
       </c>
+      <c r="I11" s="29" t="s">
+        <v>65</v>
+      </c>
       <c r="J11" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="K11" s="30"/>
-      <c r="L11" s="30"/>
-      <c r="M11" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="N11" s="27"/>
-      <c r="O11" s="27"/>
-      <c r="P11" s="27"/>
+        <v>66</v>
+      </c>
+      <c r="K11" s="32"/>
+      <c r="L11" s="32"/>
+      <c r="M11" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="N11" s="29"/>
+      <c r="O11" s="29"/>
+      <c r="P11" s="29"/>
     </row>
     <row r="12" spans="1:14">
       <c r="A12" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D12" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E12" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H12" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I12" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="K12" s="29"/>
-      <c r="L12" s="29"/>
+        <v>71</v>
+      </c>
+      <c r="K12" s="31"/>
+      <c r="L12" s="31"/>
       <c r="M12" t="b">
         <v>1</v>
       </c>
@@ -2096,25 +2131,25 @@
     </row>
     <row r="13" spans="1:14">
       <c r="A13" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D13" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E13" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I13" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="K13" s="29"/>
-      <c r="L13" s="29"/>
+        <v>75</v>
+      </c>
+      <c r="K13" s="31"/>
+      <c r="L13" s="31"/>
       <c r="M13" t="b">
         <v>1</v>
       </c>
@@ -2125,25 +2160,25 @@
     <row r="14" spans="1:13">
       <c r="A14" s="1"/>
       <c r="D14" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E14" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F14" s="21" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H14" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I14" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="K14" s="29"/>
-      <c r="L14" s="29"/>
+        <v>80</v>
+      </c>
+      <c r="K14" s="31"/>
+      <c r="L14" s="31"/>
       <c r="M14" t="b">
         <v>1</v>
       </c>
@@ -2153,44 +2188,44 @@
       <c r="B15" s="24"/>
       <c r="C15" s="24"/>
       <c r="D15" s="25" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E15" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="F15" s="28"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="27"/>
-      <c r="I15" s="27"/>
+        <v>81</v>
+      </c>
+      <c r="F15" s="30"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="29"/>
+      <c r="I15" s="29"/>
       <c r="J15" s="3"/>
-      <c r="K15" s="30"/>
-      <c r="L15" s="30"/>
-      <c r="M15" s="27"/>
-      <c r="N15" s="27"/>
-      <c r="O15" s="27"/>
-      <c r="P15" s="27"/>
+      <c r="K15" s="32"/>
+      <c r="L15" s="32"/>
+      <c r="M15" s="29"/>
+      <c r="N15" s="29"/>
+      <c r="O15" s="29"/>
+      <c r="P15" s="29"/>
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D16" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E16" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H16" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="I16" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="K16" s="29"/>
-      <c r="L16" s="29"/>
+        <v>87</v>
+      </c>
+      <c r="K16" s="31"/>
+      <c r="L16" s="31"/>
       <c r="M16" t="b">
         <v>1</v>
       </c>
@@ -2200,25 +2235,25 @@
     </row>
     <row r="17" spans="1:14">
       <c r="A17" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D17" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E17" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H17" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="I17" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="K17" s="29"/>
-      <c r="L17" s="29"/>
+        <v>92</v>
+      </c>
+      <c r="K17" s="31"/>
+      <c r="L17" s="31"/>
       <c r="M17" t="b">
         <v>1</v>
       </c>
@@ -2226,62 +2261,158 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:14">
-      <c r="A18" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="D18" t="s">
-        <v>92</v>
-      </c>
-      <c r="E18" t="s">
-        <v>18</v>
-      </c>
-      <c r="H18" t="s">
+    <row r="18" spans="1:17">
+      <c r="A18" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="B18" s="27"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27" t="s">
         <v>93</v>
       </c>
-      <c r="I18" t="s">
+      <c r="E18" s="27" t="s">
         <v>94</v>
+      </c>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="I18" s="27" t="s">
+        <v>95</v>
       </c>
       <c r="J18" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="K18" s="29"/>
-      <c r="L18" s="29"/>
-      <c r="M18" t="b">
-        <v>1</v>
-      </c>
-      <c r="N18" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12">
-      <c r="A19" s="1"/>
-      <c r="K19" s="29"/>
-      <c r="L19" s="29"/>
-    </row>
-    <row r="20" spans="1:12">
-      <c r="A20" s="1"/>
-      <c r="K20" s="29"/>
-      <c r="L20" s="29"/>
-    </row>
-    <row r="21" spans="1:12">
-      <c r="A21" s="1"/>
-      <c r="K21" s="29"/>
-      <c r="L21" s="29"/>
+      <c r="K18" s="33"/>
+      <c r="L18" s="33"/>
+      <c r="M18" s="27"/>
+      <c r="N18" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="O18" s="27"/>
+      <c r="P18" s="27"/>
+      <c r="Q18" s="27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17">
+      <c r="A19" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="B19" s="27"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="E19" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="F19" s="27"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="27" t="s">
+        <v>97</v>
+      </c>
+      <c r="I19" s="27" t="s">
+        <v>97</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="K19" s="33"/>
+      <c r="L19" s="33"/>
+      <c r="M19" s="27"/>
+      <c r="N19" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="O19" s="27"/>
+      <c r="P19" s="27"/>
+      <c r="Q19" s="27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17">
+      <c r="A20" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="B20" s="27"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="27" t="s">
+        <v>98</v>
+      </c>
+      <c r="E20" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="F20" s="27"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="I20" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="K20" s="33"/>
+      <c r="L20" s="33"/>
+      <c r="M20" s="27"/>
+      <c r="N20" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="O20" s="27"/>
+      <c r="P20" s="27"/>
+      <c r="Q20" s="27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
+      <c r="A21" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D21" t="s">
+        <v>100</v>
+      </c>
+      <c r="E21" t="s">
+        <v>19</v>
+      </c>
+      <c r="H21" t="s">
+        <v>101</v>
+      </c>
+      <c r="I21" t="s">
+        <v>102</v>
+      </c>
+      <c r="J21" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="K21" s="31"/>
+      <c r="L21" s="31"/>
+      <c r="M21" t="b">
+        <v>1</v>
+      </c>
+      <c r="N21" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="22" spans="1:12">
       <c r="A22" s="1"/>
-      <c r="K22" s="29"/>
-      <c r="L22" s="29"/>
-    </row>
-    <row r="23" spans="1:1">
+      <c r="K22" s="31"/>
+      <c r="L22" s="31"/>
+    </row>
+    <row r="23" spans="1:12">
       <c r="A23" s="1"/>
-    </row>
-    <row r="24" spans="1:1">
+      <c r="K23" s="31"/>
+      <c r="L23" s="31"/>
+    </row>
+    <row r="24" spans="1:12">
       <c r="A24" s="1"/>
-    </row>
-    <row r="25" spans="1:1">
+      <c r="K24" s="31"/>
+      <c r="L24" s="31"/>
+    </row>
+    <row r="25" spans="1:12">
       <c r="A25" s="1"/>
+      <c r="K25" s="31"/>
+      <c r="L25" s="31"/>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" s="1"/>
@@ -2306,6 +2437,15 @@
     </row>
     <row r="33" spans="1:1">
       <c r="A33" s="1"/>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" s="1"/>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" s="1"/>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7875" right="0.7875" top="0.7875" bottom="0.7875" header="0.39375" footer="0.39375"/>
@@ -2337,7 +2477,7 @@
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="C1" t="s">
         <v>7</v>
@@ -2354,366 +2494,366 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="B2" s="1" t="b">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="D2" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="B3" s="1" t="b">
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="D3" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="5" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="F4" s="5"/>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="5" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="F5" s="5"/>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="5" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="E6" s="18" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="F6" s="19" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
       <c r="E8" s="20" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="E9" s="20" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="E10" s="20" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="E11" s="20" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="E12" s="20" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="E13" s="20" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="E14" s="20" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="C15" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="D15" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
     </row>
     <row r="16" s="4" customFormat="1" spans="1:5">
       <c r="A16" s="10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
     </row>
     <row r="17" s="4" customFormat="1" spans="1:5">
       <c r="A17" s="10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
     </row>
     <row r="18" s="4" customFormat="1" spans="1:5">
       <c r="A18" s="10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
     </row>
     <row r="19" s="4" customFormat="1" spans="1:5">
       <c r="A19" s="10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>169</v>
+        <v>177</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>170</v>
+        <v>178</v>
       </c>
     </row>
     <row r="20" s="4" customFormat="1" spans="1:5">
       <c r="A20" s="10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>173</v>
+        <v>181</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>174</v>
+        <v>182</v>
       </c>
     </row>
     <row r="21" s="4" customFormat="1" spans="1:5">
       <c r="A21" s="10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>176</v>
+        <v>184</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
     </row>
     <row r="22" s="4" customFormat="1" spans="1:5">
       <c r="A22" s="10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -2882,48 +3022,48 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
       <c r="C1" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
       <c r="E1" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>189</v>
+        <v>197</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="B2" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="C2" t="s">
-        <v>192</v>
+        <v>200</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
       <c r="E2" s="1">
         <v>1</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Add new columns to core forms (education and religion) - Add CoreFormColumnOptions domain model and synchronization from the server - Updating HForms and UI   - add education and religion to member enu, ext inmig, and inmig forms   - update labels, numbering, etc
</commit_message>
<xml_diff>
--- a/app/src/main/res/raw/change_head_form.xlsx
+++ b/app/src/main/res/raw/change_head_form.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="18420" yWindow="5850" windowWidth="9210" windowHeight="6465" tabRatio="500"/>
+    <workbookView windowWidth="27795" windowHeight="12270" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="columns" sheetId="1" r:id="rId1"/>
@@ -307,13 +307,13 @@
     <t>username</t>
   </si>
   <si>
-    <t>6.1. Collected By Fieldworker</t>
-  </si>
-  <si>
-    <t>6.1. Código do Inquiridor</t>
-  </si>
-  <si>
-    <t>6.1. Code de l'enquêteur</t>
+    <t>Collected By Fieldworker</t>
+  </si>
+  <si>
+    <t>Código do Inquiridor</t>
+  </si>
+  <si>
+    <t>Code de l'enquêteur</t>
   </si>
   <si>
     <t>collectedDate</t>
@@ -322,13 +322,13 @@
     <t>timestamp</t>
   </si>
   <si>
-    <t>6.2. Collected Date</t>
-  </si>
-  <si>
-    <t>6.2. Data da Visita</t>
-  </si>
-  <si>
-    <t>6.2. Date de la visite</t>
+    <t>Collected Date</t>
+  </si>
+  <si>
+    <t>Data da Visita</t>
+  </si>
+  <si>
+    <t>Date de la visite</t>
   </si>
   <si>
     <t>collectedDeviceId</t>
@@ -666,10 +666,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -718,21 +718,29 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF800080"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Arial"/>
       <charset val="134"/>
@@ -740,14 +748,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -761,69 +770,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -839,7 +788,65 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -848,13 +855,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -898,31 +898,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -934,31 +1060,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -968,122 +1082,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="10">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -1109,9 +1109,77 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1134,48 +1202,7 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -1196,6 +1223,30 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -1204,155 +1255,166 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1402,6 +1464,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1413,10 +1478,15 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1424,12 +1494,21 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1747,7 +1826,7 @@
   <dimension ref="A1:Q36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18:M20"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="12.75"/>
@@ -1757,8 +1836,8 @@
     <col min="3" max="3" width="14.1809523809524" customWidth="1"/>
     <col min="4" max="4" width="20.1809523809524" customWidth="1"/>
     <col min="5" max="5" width="11.7238095238095" customWidth="1"/>
-    <col min="6" max="6" width="12" style="21" customWidth="1"/>
-    <col min="7" max="7" width="20" style="21" customWidth="1"/>
+    <col min="6" max="6" width="12" style="24" customWidth="1"/>
+    <col min="7" max="7" width="20" style="24" customWidth="1"/>
     <col min="8" max="8" width="51.5428571428571" customWidth="1"/>
     <col min="9" max="10" width="55" customWidth="1"/>
     <col min="11" max="12" width="16.2666666666667" customWidth="1"/>
@@ -1783,10 +1862,10 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="24" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -1810,13 +1889,13 @@
       <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="21" t="s">
+      <c r="O1" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="34" t="s">
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="34" t="s">
+      <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1826,13 +1905,13 @@
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="22" t="s">
+      <c r="H2" s="25" t="s">
         <v>20</v>
       </c>
       <c r="I2" t="s">
@@ -1849,7 +1928,7 @@
       <c r="N2" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="O2" s="21"/>
+      <c r="O2" s="24"/>
     </row>
     <row r="3" spans="1:15">
       <c r="A3" s="1" t="s">
@@ -1857,13 +1936,13 @@
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="22" t="s">
+      <c r="H3" s="25" t="s">
         <v>24</v>
       </c>
       <c r="I3" t="s">
@@ -1880,7 +1959,7 @@
       <c r="N3" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="O3" s="21"/>
+      <c r="O3" s="24"/>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="1" t="s">
@@ -1901,8 +1980,8 @@
       <c r="J4" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="K4" s="31"/>
-      <c r="L4" s="31"/>
+      <c r="K4" s="38"/>
+      <c r="L4" s="38"/>
       <c r="M4" t="b">
         <v>1</v>
       </c>
@@ -1929,8 +2008,8 @@
       <c r="J5" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="K5" s="31"/>
-      <c r="L5" s="31"/>
+      <c r="K5" s="38"/>
+      <c r="L5" s="38"/>
       <c r="M5" t="b">
         <v>1</v>
       </c>
@@ -1957,8 +2036,8 @@
       <c r="J6" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="K6" s="31"/>
-      <c r="L6" s="31"/>
+      <c r="K6" s="38"/>
+      <c r="L6" s="38"/>
       <c r="M6" t="b">
         <v>1</v>
       </c>
@@ -1985,8 +2064,8 @@
       <c r="J7" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="K7" s="31"/>
-      <c r="L7" s="31"/>
+      <c r="K7" s="38"/>
+      <c r="L7" s="38"/>
       <c r="M7" t="b">
         <v>1</v>
       </c>
@@ -2011,8 +2090,8 @@
       <c r="J8" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="K8" s="31"/>
-      <c r="L8" s="31"/>
+      <c r="K8" s="38"/>
+      <c r="L8" s="38"/>
       <c r="M8" t="b">
         <v>1</v>
       </c>
@@ -2025,7 +2104,7 @@
       <c r="E9" t="s">
         <v>51</v>
       </c>
-      <c r="F9" s="21" t="s">
+      <c r="F9" s="24" t="s">
         <v>52</v>
       </c>
       <c r="H9" t="s">
@@ -2037,8 +2116,8 @@
       <c r="J9" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="K9" s="31"/>
-      <c r="L9" s="31"/>
+      <c r="K9" s="38"/>
+      <c r="L9" s="38"/>
       <c r="M9" t="b">
         <v>1</v>
       </c>
@@ -2060,8 +2139,8 @@
       <c r="J10" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="K10" s="31"/>
-      <c r="L10" s="31"/>
+      <c r="K10" s="38"/>
+      <c r="L10" s="38"/>
       <c r="M10" t="b">
         <v>1</v>
       </c>
@@ -2070,36 +2149,36 @@
       </c>
     </row>
     <row r="11" spans="1:16">
-      <c r="A11" s="23"/>
-      <c r="B11" s="24"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="25" t="s">
+      <c r="A11" s="26"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="E11" s="25" t="s">
+      <c r="E11" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="F11" s="28"/>
-      <c r="G11" s="28" t="s">
+      <c r="F11" s="32"/>
+      <c r="G11" s="32" t="s">
         <v>63</v>
       </c>
-      <c r="H11" s="29" t="s">
+      <c r="H11" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="I11" s="29" t="s">
+      <c r="I11" s="33" t="s">
         <v>65</v>
       </c>
       <c r="J11" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="K11" s="32"/>
-      <c r="L11" s="32"/>
-      <c r="M11" s="29" t="b">
-        <v>1</v>
-      </c>
-      <c r="N11" s="29"/>
-      <c r="O11" s="29"/>
-      <c r="P11" s="29"/>
+      <c r="K11" s="39"/>
+      <c r="L11" s="39"/>
+      <c r="M11" s="33" t="b">
+        <v>1</v>
+      </c>
+      <c r="N11" s="33"/>
+      <c r="O11" s="33"/>
+      <c r="P11" s="33"/>
     </row>
     <row r="12" spans="1:14">
       <c r="A12" s="1" t="s">
@@ -2120,8 +2199,8 @@
       <c r="J12" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="K12" s="31"/>
-      <c r="L12" s="31"/>
+      <c r="K12" s="38"/>
+      <c r="L12" s="38"/>
       <c r="M12" t="b">
         <v>1</v>
       </c>
@@ -2148,8 +2227,8 @@
       <c r="J13" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="K13" s="31"/>
-      <c r="L13" s="31"/>
+      <c r="K13" s="38"/>
+      <c r="L13" s="38"/>
       <c r="M13" t="b">
         <v>1</v>
       </c>
@@ -2165,7 +2244,7 @@
       <c r="E14" t="s">
         <v>77</v>
       </c>
-      <c r="F14" s="21" t="s">
+      <c r="F14" s="24" t="s">
         <v>61</v>
       </c>
       <c r="H14" t="s">
@@ -2177,242 +2256,248 @@
       <c r="J14" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="K14" s="31"/>
-      <c r="L14" s="31"/>
+      <c r="K14" s="38"/>
+      <c r="L14" s="38"/>
       <c r="M14" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:16">
-      <c r="A15" s="23"/>
-      <c r="B15" s="24"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="25" t="s">
+      <c r="A15" s="26"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="E15" s="25" t="s">
+      <c r="E15" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="F15" s="30"/>
-      <c r="G15" s="30"/>
-      <c r="H15" s="29"/>
-      <c r="I15" s="29"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="32"/>
-      <c r="L15" s="32"/>
-      <c r="M15" s="29"/>
-      <c r="N15" s="29"/>
-      <c r="O15" s="29"/>
-      <c r="P15" s="29"/>
-    </row>
-    <row r="16" spans="1:14">
-      <c r="A16" s="1" t="s">
+      <c r="F15" s="34"/>
+      <c r="G15" s="34"/>
+      <c r="H15" s="33"/>
+      <c r="I15" s="33"/>
+      <c r="J15" s="40"/>
+      <c r="K15" s="39"/>
+      <c r="L15" s="39"/>
+      <c r="M15" s="33"/>
+      <c r="N15" s="33"/>
+      <c r="O15" s="33"/>
+      <c r="P15" s="33"/>
+    </row>
+    <row r="16" s="21" customFormat="1" spans="1:14">
+      <c r="A16" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="H16" t="s">
+      <c r="F16" s="35"/>
+      <c r="G16" s="35"/>
+      <c r="H16" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="I16" t="s">
+      <c r="I16" s="21" t="s">
         <v>86</v>
       </c>
       <c r="J16" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="K16" s="31"/>
-      <c r="L16" s="31"/>
-      <c r="M16" t="b">
-        <v>1</v>
-      </c>
-      <c r="N16" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14">
-      <c r="A17" s="1" t="s">
+      <c r="K16" s="41"/>
+      <c r="L16" s="41"/>
+      <c r="M16" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="N16" s="21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" s="22" customFormat="1" spans="1:14">
+      <c r="A17" s="30" t="s">
         <v>82</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="22" t="s">
         <v>89</v>
       </c>
-      <c r="H17" t="s">
+      <c r="F17" s="36"/>
+      <c r="G17" s="36"/>
+      <c r="H17" s="22" t="s">
         <v>90</v>
       </c>
-      <c r="I17" t="s">
+      <c r="I17" s="22" t="s">
         <v>91</v>
       </c>
       <c r="J17" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="K17" s="31"/>
-      <c r="L17" s="31"/>
-      <c r="M17" t="b">
-        <v>1</v>
-      </c>
-      <c r="N17" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17">
-      <c r="A18" s="26" t="s">
+      <c r="K17" s="42"/>
+      <c r="L17" s="42"/>
+      <c r="M17" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="N17" s="22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" s="22" customFormat="1" spans="1:17">
+      <c r="A18" s="30" t="s">
         <v>82</v>
       </c>
-      <c r="B18" s="27"/>
-      <c r="C18" s="27"/>
-      <c r="D18" s="27" t="s">
+      <c r="B18" s="22"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="E18" s="27" t="s">
+      <c r="E18" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="F18" s="27"/>
-      <c r="G18" s="27"/>
-      <c r="H18" s="27" t="s">
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="22" t="s">
         <v>95</v>
       </c>
-      <c r="I18" s="27" t="s">
+      <c r="I18" s="22" t="s">
         <v>95</v>
       </c>
       <c r="J18" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="K18" s="33"/>
-      <c r="L18" s="33"/>
-      <c r="M18" s="27"/>
-      <c r="N18" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="O18" s="27"/>
-      <c r="P18" s="27"/>
-      <c r="Q18" s="27" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17">
-      <c r="A19" s="26" t="s">
+      <c r="K18" s="42"/>
+      <c r="L18" s="42"/>
+      <c r="M18" s="22"/>
+      <c r="N18" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="O18" s="22"/>
+      <c r="P18" s="22"/>
+      <c r="Q18" s="22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" s="22" customFormat="1" spans="1:17">
+      <c r="A19" s="30" t="s">
         <v>82</v>
       </c>
-      <c r="B19" s="27"/>
-      <c r="C19" s="27"/>
-      <c r="D19" s="27" t="s">
+      <c r="B19" s="22"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22" t="s">
         <v>96</v>
       </c>
-      <c r="E19" s="27" t="s">
+      <c r="E19" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="F19" s="27"/>
-      <c r="G19" s="27"/>
-      <c r="H19" s="27" t="s">
+      <c r="F19" s="22"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="22" t="s">
         <v>97</v>
       </c>
-      <c r="I19" s="27" t="s">
+      <c r="I19" s="22" t="s">
         <v>97</v>
       </c>
       <c r="J19" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="K19" s="33"/>
-      <c r="L19" s="33"/>
-      <c r="M19" s="27"/>
-      <c r="N19" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="O19" s="27"/>
-      <c r="P19" s="27"/>
-      <c r="Q19" s="27" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17">
-      <c r="A20" s="26" t="s">
+      <c r="K19" s="42"/>
+      <c r="L19" s="42"/>
+      <c r="M19" s="22"/>
+      <c r="N19" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="O19" s="22"/>
+      <c r="P19" s="22"/>
+      <c r="Q19" s="22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" s="22" customFormat="1" spans="1:17">
+      <c r="A20" s="30" t="s">
         <v>82</v>
       </c>
-      <c r="B20" s="27"/>
-      <c r="C20" s="27"/>
-      <c r="D20" s="27" t="s">
+      <c r="B20" s="22"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22" t="s">
         <v>98</v>
       </c>
-      <c r="E20" s="27" t="s">
+      <c r="E20" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="F20" s="27"/>
-      <c r="G20" s="27"/>
-      <c r="H20" s="27" t="s">
+      <c r="F20" s="22"/>
+      <c r="G20" s="22"/>
+      <c r="H20" s="22" t="s">
         <v>99</v>
       </c>
-      <c r="I20" s="27" t="s">
+      <c r="I20" s="22" t="s">
         <v>99</v>
       </c>
       <c r="J20" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="K20" s="33"/>
-      <c r="L20" s="33"/>
-      <c r="M20" s="27"/>
-      <c r="N20" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="O20" s="27"/>
-      <c r="P20" s="27"/>
-      <c r="Q20" s="27" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14">
-      <c r="A21" s="1" t="s">
+      <c r="K20" s="42"/>
+      <c r="L20" s="42"/>
+      <c r="M20" s="22"/>
+      <c r="N20" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="O20" s="22"/>
+      <c r="P20" s="22"/>
+      <c r="Q20" s="22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" s="23" customFormat="1" spans="1:14">
+      <c r="A21" s="31" t="s">
         <v>82</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="H21" t="s">
+      <c r="F21" s="37"/>
+      <c r="G21" s="37"/>
+      <c r="H21" s="23" t="s">
         <v>101</v>
       </c>
-      <c r="I21" t="s">
+      <c r="I21" s="23" t="s">
         <v>102</v>
       </c>
       <c r="J21" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="K21" s="31"/>
-      <c r="L21" s="31"/>
-      <c r="M21" t="b">
-        <v>1</v>
-      </c>
-      <c r="N21" t="b">
+      <c r="K21" s="43"/>
+      <c r="L21" s="43"/>
+      <c r="M21" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="N21" s="23" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:12">
       <c r="A22" s="1"/>
-      <c r="K22" s="31"/>
-      <c r="L22" s="31"/>
+      <c r="K22" s="38"/>
+      <c r="L22" s="38"/>
     </row>
     <row r="23" spans="1:12">
       <c r="A23" s="1"/>
-      <c r="K23" s="31"/>
-      <c r="L23" s="31"/>
+      <c r="K23" s="38"/>
+      <c r="L23" s="38"/>
     </row>
     <row r="24" spans="1:12">
       <c r="A24" s="1"/>
-      <c r="K24" s="31"/>
-      <c r="L24" s="31"/>
+      <c r="K24" s="38"/>
+      <c r="L24" s="38"/>
     </row>
     <row r="25" spans="1:12">
       <c r="A25" s="1"/>
-      <c r="K25" s="31"/>
-      <c r="L25" s="31"/>
+      <c r="K25" s="38"/>
+      <c r="L25" s="38"/>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" s="1"/>

</xml_diff>

<commit_message>
- Add more checks for cross-checking dates to previous Residency and HeadRelationship on FormUtil   - ChangeHead, Death, Migrations, Enumeration, MaritalRelationship and Pregnancy Outcome FormUtils - Allow Change Head on a Households without Head - Put LoadingDialog on ShowCollectedDataActivity for loading that takes too long - Fix Member still appearing after Death - Add more retries when checking if ODK Form is Finalized - Fix birthplaces on pregnancy_outcome raw form
</commit_message>
<xml_diff>
--- a/app/src/main/res/raw/change_head_form.xlsx
+++ b/app/src/main/res/raw/change_head_form.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27795" windowHeight="12270" tabRatio="500"/>
+    <workbookView windowWidth="27795" windowHeight="12195" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="columns" sheetId="1" r:id="rId1"/>
@@ -709,16 +709,16 @@
       <charset val="134"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF3F3F76"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -733,53 +733,14 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Arial"/>
       <charset val="134"/>
@@ -796,7 +757,37 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -810,22 +801,29 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Arial"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF9C0006"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -838,23 +836,25 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -898,67 +898,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -970,115 +1078,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1170,21 +1170,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -1208,6 +1193,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -1219,6 +1213,41 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1237,180 +1266,151 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="25" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="177" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="29" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1825,8 +1825,8 @@
   <sheetPr/>
   <dimension ref="A1:Q36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="12.75"/>
@@ -1982,9 +1982,7 @@
       </c>
       <c r="K4" s="38"/>
       <c r="L4" s="38"/>
-      <c r="M4" t="b">
-        <v>1</v>
-      </c>
+      <c r="M4"/>
       <c r="N4" t="b">
         <v>1</v>
       </c>
@@ -2010,9 +2008,7 @@
       </c>
       <c r="K5" s="38"/>
       <c r="L5" s="38"/>
-      <c r="M5" t="b">
-        <v>1</v>
-      </c>
+      <c r="M5"/>
       <c r="N5" t="b">
         <v>1</v>
       </c>
@@ -2348,16 +2344,12 @@
       <c r="A18" s="30" t="s">
         <v>82</v>
       </c>
-      <c r="B18" s="22"/>
-      <c r="C18" s="22"/>
       <c r="D18" s="22" t="s">
         <v>93</v>
       </c>
       <c r="E18" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="F18" s="22"/>
-      <c r="G18" s="22"/>
       <c r="H18" s="22" t="s">
         <v>95</v>
       </c>
@@ -2369,12 +2361,9 @@
       </c>
       <c r="K18" s="42"/>
       <c r="L18" s="42"/>
-      <c r="M18" s="22"/>
       <c r="N18" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="O18" s="22"/>
-      <c r="P18" s="22"/>
       <c r="Q18" s="22" t="b">
         <v>1</v>
       </c>
@@ -2383,16 +2372,12 @@
       <c r="A19" s="30" t="s">
         <v>82</v>
       </c>
-      <c r="B19" s="22"/>
-      <c r="C19" s="22"/>
       <c r="D19" s="22" t="s">
         <v>96</v>
       </c>
       <c r="E19" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="F19" s="22"/>
-      <c r="G19" s="22"/>
       <c r="H19" s="22" t="s">
         <v>97</v>
       </c>
@@ -2404,12 +2389,9 @@
       </c>
       <c r="K19" s="42"/>
       <c r="L19" s="42"/>
-      <c r="M19" s="22"/>
       <c r="N19" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="O19" s="22"/>
-      <c r="P19" s="22"/>
       <c r="Q19" s="22" t="b">
         <v>1</v>
       </c>
@@ -2418,16 +2400,12 @@
       <c r="A20" s="30" t="s">
         <v>82</v>
       </c>
-      <c r="B20" s="22"/>
-      <c r="C20" s="22"/>
       <c r="D20" s="22" t="s">
         <v>98</v>
       </c>
       <c r="E20" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="F20" s="22"/>
-      <c r="G20" s="22"/>
       <c r="H20" s="22" t="s">
         <v>99</v>
       </c>
@@ -2439,12 +2417,9 @@
       </c>
       <c r="K20" s="42"/>
       <c r="L20" s="42"/>
-      <c r="M20" s="22"/>
       <c r="N20" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="O20" s="22"/>
-      <c r="P20" s="22"/>
       <c r="Q20" s="22" t="b">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
- Add support to Ahmaric Ethiopia Language   - Create a translated values-am/strings.xml   - Update Login password field to support input in ahmaric   - Add translations to HDS Core Forms
</commit_message>
<xml_diff>
--- a/app/src/main/res/raw/change_head_form.xlsx
+++ b/app/src/main/res/raw/change_head_form.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27795" windowHeight="12195" tabRatio="500"/>
+    <workbookView windowWidth="27795" windowHeight="12195" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="columns" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <author>paul</author>
   </authors>
   <commentList>
-    <comment ref="F1" authorId="0">
+    <comment ref="G1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="246">
   <si>
     <t>group</t>
   </si>
@@ -82,6 +82,9 @@
     <t>label::fr</t>
   </si>
   <si>
+    <t>label::am</t>
+  </si>
+  <si>
     <t>default_value</t>
   </si>
   <si>
@@ -121,6 +124,9 @@
     <t>1.0. Code de visite</t>
   </si>
   <si>
+    <t xml:space="preserve">1.0. የጉብኝት ኮድ  </t>
+  </si>
+  <si>
     <t>householdCode</t>
   </si>
   <si>
@@ -133,6 +139,9 @@
     <t>1.1. Code de la maison</t>
   </si>
   <si>
+    <t xml:space="preserve">1.1. የቤተሰብ ኮድ  </t>
+  </si>
+  <si>
     <t>header2</t>
   </si>
   <si>
@@ -148,6 +157,9 @@
     <t>2.1. Code de l'ancien chef de ménage</t>
   </si>
   <si>
+    <t xml:space="preserve">2.1. የአሁኑ የቤተሰብ አለቃ ኮድ  </t>
+  </si>
+  <si>
     <t>oldHeadName</t>
   </si>
   <si>
@@ -160,6 +172,9 @@
     <t>2.2. Nom de l'ancien chef de ménage</t>
   </si>
   <si>
+    <t xml:space="preserve">2.2. የአሁኑ የቤተሰብ አለቃ ስም  </t>
+  </si>
+  <si>
     <t>newhead</t>
   </si>
   <si>
@@ -175,6 +190,9 @@
     <t>3.1. Code du nouveau chef de ménage</t>
   </si>
   <si>
+    <t xml:space="preserve">3.1. አዲሱ የቤተሰብ አለቃ ኮድ  </t>
+  </si>
+  <si>
     <t>newHeadName</t>
   </si>
   <si>
@@ -187,6 +205,9 @@
     <t>3.2. Nom du nouveau chef de ménage</t>
   </si>
   <si>
+    <t xml:space="preserve">3.2. አዲሱ የቤተሰብ አለቃ ስም  </t>
+  </si>
+  <si>
     <t>eventDate</t>
   </si>
   <si>
@@ -202,6 +223,9 @@
     <t>4.1. Date de l'événement?</t>
   </si>
   <si>
+    <t xml:space="preserve">4.1. የለውጡ ክስተት ቀን  </t>
+  </si>
+  <si>
     <t>reason</t>
   </si>
   <si>
@@ -220,6 +244,9 @@
     <t>4.2. Quelle est la raison du déménagement du chef de ménage?</t>
   </si>
   <si>
+    <t xml:space="preserve">4.2. የቤተሰብ አለቃን ለመቀየር ምክንያት  </t>
+  </si>
+  <si>
     <t>reasonOther</t>
   </si>
   <si>
@@ -232,6 +259,9 @@
     <t>4.2.1. Préciser le motif</t>
   </si>
   <si>
+    <t xml:space="preserve">4.2.1. ምክንያቱን ዝርዝር አሳይ  </t>
+  </si>
+  <si>
     <t>${reason} = 'OTHER'</t>
   </si>
   <si>
@@ -253,6 +283,9 @@
     <t>5. Relation des membres avec le nouveau chef de ménage</t>
   </si>
   <si>
+    <t xml:space="preserve">5. አባላትን ከአዲሱ የቤተሰብ አለቃ ጋር ያላቸው ዝምድና  </t>
+  </si>
+  <si>
     <t>newheadrelat</t>
   </si>
   <si>
@@ -268,6 +301,9 @@
     <t>5.1. Code du membre</t>
   </si>
   <si>
+    <t xml:space="preserve">5.1. የአባል ኮድ  </t>
+  </si>
+  <si>
     <t>newMemberName</t>
   </si>
   <si>
@@ -280,6 +316,9 @@
     <t>5.2. Nom du membre</t>
   </si>
   <si>
+    <t xml:space="preserve">5.2. የአባል ስም  </t>
+  </si>
+  <si>
     <t>newRelationshipType</t>
   </si>
   <si>
@@ -295,6 +334,9 @@
     <t>5.3. Relation avec le nouveau chef de ménage</t>
   </si>
   <si>
+    <t xml:space="preserve">5.3. ከአዲሱ የቤተሰብ አለቃ ጋር ያለው ዝምድና  </t>
+  </si>
+  <si>
     <t>end repeat</t>
   </si>
   <si>
@@ -316,6 +358,9 @@
     <t>Code de l'enquêteur</t>
   </si>
   <si>
+    <t xml:space="preserve">በመረጃ ባለሞያ ተከሰተ  </t>
+  </si>
+  <si>
     <t>collectedDate</t>
   </si>
   <si>
@@ -331,6 +376,9 @@
     <t>Date de la visite</t>
   </si>
   <si>
+    <t xml:space="preserve">ቀን ተከሰተ  </t>
+  </si>
+  <si>
     <t>collectedDeviceId</t>
   </si>
   <si>
@@ -340,18 +388,27 @@
     <t>Device Id</t>
   </si>
   <si>
+    <t xml:space="preserve">የመሳሪያ መታወቂያ  </t>
+  </si>
+  <si>
     <t>collectedHouseholdId</t>
   </si>
   <si>
     <t>Collected Household Id</t>
   </si>
   <si>
+    <t xml:space="preserve">የተከሰተው የቤተሰብ መታወቂያ  </t>
+  </si>
+  <si>
     <t>collectedMemberId</t>
   </si>
   <si>
     <t>Collected Member Id</t>
   </si>
   <si>
+    <t xml:space="preserve">የተከሰተው የአባል መታወቂያ  </t>
+  </si>
+  <si>
     <t>modules</t>
   </si>
   <si>
@@ -364,6 +421,9 @@
     <t>Accès aux modules autorisé</t>
   </si>
   <si>
+    <t>ለመድረሻዎች የተፈቀደ መዳረሻ</t>
+  </si>
+  <si>
     <t>value</t>
   </si>
   <si>
@@ -379,6 +439,9 @@
     <t>Oui</t>
   </si>
   <si>
+    <t xml:space="preserve">አዎን  </t>
+  </si>
+  <si>
     <t>No</t>
   </si>
   <si>
@@ -388,6 +451,9 @@
     <t>Non</t>
   </si>
   <si>
+    <t xml:space="preserve">አይደለም  </t>
+  </si>
+  <si>
     <t>genders</t>
   </si>
   <si>
@@ -403,6 +469,9 @@
     <t>Masculin</t>
   </si>
   <si>
+    <t xml:space="preserve">ወንድ  </t>
+  </si>
+  <si>
     <t>F</t>
   </si>
   <si>
@@ -415,6 +484,9 @@
     <t>Féminin</t>
   </si>
   <si>
+    <t xml:space="preserve">ሴት  </t>
+  </si>
+  <si>
     <t>HOH</t>
   </si>
   <si>
@@ -427,6 +499,9 @@
     <t>Chef de ménage</t>
   </si>
   <si>
+    <t xml:space="preserve">የቤተሰብ አለቃ  </t>
+  </si>
+  <si>
     <t>true</t>
   </si>
   <si>
@@ -442,6 +517,9 @@
     <t>Conjoint</t>
   </si>
   <si>
+    <t xml:space="preserve">ባል/ሚስት  </t>
+  </si>
+  <si>
     <t>SON</t>
   </si>
   <si>
@@ -454,6 +532,9 @@
     <t>Fils/Fille</t>
   </si>
   <si>
+    <t xml:space="preserve">ልጅ  </t>
+  </si>
+  <si>
     <t>BRO</t>
   </si>
   <si>
@@ -466,6 +547,9 @@
     <t>Frère/Sœur</t>
   </si>
   <si>
+    <t xml:space="preserve">እህት/ወንድም  </t>
+  </si>
+  <si>
     <t>PAR</t>
   </si>
   <si>
@@ -478,6 +562,9 @@
     <t>Père/Mère</t>
   </si>
   <si>
+    <t xml:space="preserve">ወላጅ  </t>
+  </si>
+  <si>
     <t>GCH</t>
   </si>
   <si>
@@ -490,6 +577,9 @@
     <t>Petits-enfants</t>
   </si>
   <si>
+    <t xml:space="preserve">የልጅ ልጅ  </t>
+  </si>
+  <si>
     <t>NOR</t>
   </si>
   <si>
@@ -502,6 +592,9 @@
     <t>Aucun lien</t>
   </si>
   <si>
+    <t xml:space="preserve">ዝምድና የለውም  </t>
+  </si>
+  <si>
     <t>OTH</t>
   </si>
   <si>
@@ -514,6 +607,9 @@
     <t>Autre parent</t>
   </si>
   <si>
+    <t xml:space="preserve">ሌላ ዘመድ  </t>
+  </si>
+  <si>
     <t>DNK</t>
   </si>
   <si>
@@ -526,6 +622,9 @@
     <t>Ne sait pas</t>
   </si>
   <si>
+    <t xml:space="preserve">አላውቅም  </t>
+  </si>
+  <si>
     <t>migtypes</t>
   </si>
   <si>
@@ -541,6 +640,9 @@
     <t>Immigration interne</t>
   </si>
   <si>
+    <t xml:space="preserve">ውስጣዊ እንቅስቃሴ  </t>
+  </si>
+  <si>
     <t>RESIDENCY_CHANGE</t>
   </si>
   <si>
@@ -553,6 +655,9 @@
     <t>Par changement de résidence</t>
   </si>
   <si>
+    <t xml:space="preserve">የመኖሪያ ሁኔታ ለውጥ  </t>
+  </si>
+  <si>
     <t>OLD_AGE</t>
   </si>
   <si>
@@ -565,6 +670,9 @@
     <t>Âge avancé de l'ancien chef</t>
   </si>
   <si>
+    <t xml:space="preserve">የቀድሞው አለቃ ዕድሜ በመብረቅ  </t>
+  </si>
+  <si>
     <t>DIVORCE</t>
   </si>
   <si>
@@ -577,6 +685,9 @@
     <t>Divorce/Séparation</t>
   </si>
   <si>
+    <t xml:space="preserve">ፍቺ ወይም መለያየት  </t>
+  </si>
+  <si>
     <t>WORK</t>
   </si>
   <si>
@@ -589,6 +700,9 @@
     <t>Emploi</t>
   </si>
   <si>
+    <t xml:space="preserve">ስራ  </t>
+  </si>
+  <si>
     <t>HEALTH_REASONS</t>
   </si>
   <si>
@@ -601,6 +715,9 @@
     <t>Raisons de santé</t>
   </si>
   <si>
+    <t xml:space="preserve">የጤና ምክንያቶች  </t>
+  </si>
+  <si>
     <t>DEATH</t>
   </si>
   <si>
@@ -613,6 +730,9 @@
     <t>Décès</t>
   </si>
   <si>
+    <t xml:space="preserve">ሞት  </t>
+  </si>
+  <si>
     <t>OTHER</t>
   </si>
   <si>
@@ -625,6 +745,9 @@
     <t>Autres raisons</t>
   </si>
   <si>
+    <t>ሌሎች ምክንያቶች</t>
+  </si>
+  <si>
     <t>form_id</t>
   </si>
   <si>
@@ -637,6 +760,9 @@
     <t>form_name::fr</t>
   </si>
   <si>
+    <t>form_name::am</t>
+  </si>
+  <si>
     <t>form_version</t>
   </si>
   <si>
@@ -656,6 +782,9 @@
   </si>
   <si>
     <t>Changement du chef de ménage</t>
+  </si>
+  <si>
+    <t>የቤተሰብ አለቃ ለውጥ</t>
   </si>
   <si>
     <t>rawChangeHeadRelationship</t>
@@ -668,8 +797,8 @@
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -709,16 +838,9 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -731,16 +853,46 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Arial"/>
       <charset val="134"/>
@@ -755,7 +907,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Arial"/>
@@ -763,16 +914,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Arial"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -786,51 +936,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -844,17 +952,38 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="13"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Arial"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -871,12 +1000,18 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="0.799951170384838"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -886,13 +1021,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="0.799951170384838"/>
+        <fgColor theme="1" tint="0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="1" tint="0.499984740745262"/>
+        <fgColor theme="0" tint="-0.5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -904,7 +1057,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -916,55 +1141,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -976,24 +1165,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1006,7 +1177,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1016,74 +1217,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="16">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -1156,30 +1291,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
-        <color auto="1"/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
-        <color auto="1"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1198,6 +1320,30 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1228,15 +1374,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1251,179 +1388,164 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="6" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="13" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="29" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1437,13 +1559,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1457,34 +1579,50 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1494,21 +1632,26 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1823,10 +1966,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:Q36"/>
+  <dimension ref="A1:R36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2:K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="12.75"/>
@@ -1836,17 +1979,18 @@
     <col min="3" max="3" width="14.1809523809524" customWidth="1"/>
     <col min="4" max="4" width="20.1809523809524" customWidth="1"/>
     <col min="5" max="5" width="11.7238095238095" customWidth="1"/>
-    <col min="6" max="6" width="12" style="24" customWidth="1"/>
-    <col min="7" max="7" width="20" style="24" customWidth="1"/>
+    <col min="6" max="6" width="12" style="31" customWidth="1"/>
+    <col min="7" max="7" width="20" style="31" customWidth="1"/>
     <col min="8" max="8" width="51.5428571428571" customWidth="1"/>
     <col min="9" max="10" width="55" customWidth="1"/>
-    <col min="11" max="12" width="16.2666666666667" customWidth="1"/>
-    <col min="13" max="13" width="9.26666666666667" customWidth="1"/>
-    <col min="15" max="15" width="31" customWidth="1"/>
-    <col min="16" max="16" width="13.4571428571429" customWidth="1"/>
+    <col min="11" max="11" width="41.6666666666667" customWidth="1"/>
+    <col min="12" max="13" width="16.2666666666667" customWidth="1"/>
+    <col min="14" max="14" width="9.26666666666667" customWidth="1"/>
+    <col min="16" max="16" width="31" customWidth="1"/>
+    <col min="17" max="17" width="13.4571428571429" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:18">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1862,10 +2006,10 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="F1" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="24" t="s">
+      <c r="G1" s="31" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -1889,590 +2033,653 @@
       <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="24" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="31" t="s">
         <v>15</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:15">
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
       <c r="A2" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" s="25" t="s">
+      <c r="D2" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="25" t="s">
+      <c r="E2" s="20" t="s">
         <v>20</v>
       </c>
+      <c r="H2" s="20" t="s">
+        <v>21</v>
+      </c>
       <c r="I2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="K2" s="1"/>
+        <v>23</v>
+      </c>
+      <c r="K2" s="44" t="s">
+        <v>24</v>
+      </c>
       <c r="L2" s="1"/>
-      <c r="M2" s="1" t="b">
-        <v>1</v>
-      </c>
+      <c r="M2" s="1"/>
       <c r="N2" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="O2" s="24"/>
-    </row>
-    <row r="3" spans="1:15">
+      <c r="O2" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="P2" s="31"/>
+    </row>
+    <row r="3" spans="1:16">
       <c r="A3" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" s="25" t="s">
-        <v>24</v>
+      <c r="D3" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="20" t="s">
+        <v>26</v>
       </c>
       <c r="I3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="K3" s="1"/>
+        <v>28</v>
+      </c>
+      <c r="K3" s="44" t="s">
+        <v>29</v>
+      </c>
       <c r="L3" s="1"/>
-      <c r="M3" s="1" t="b">
-        <v>1</v>
-      </c>
+      <c r="M3" s="1"/>
       <c r="N3" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="O3" s="24"/>
-    </row>
-    <row r="4" spans="1:14">
+      <c r="O3" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="P3" s="31"/>
+    </row>
+    <row r="4" spans="1:15">
       <c r="A4" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D4" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H4" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="I4" t="s">
+        <v>33</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="K4" s="45" t="s">
+        <v>35</v>
+      </c>
+      <c r="L4" s="45"/>
+      <c r="M4" s="45"/>
+      <c r="O4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="J4" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="K4" s="38"/>
-      <c r="L4" s="38"/>
-      <c r="M4"/>
-      <c r="N4" t="b">
+      <c r="D5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" t="s">
+        <v>37</v>
+      </c>
+      <c r="I5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="K5" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="L5" s="45"/>
+      <c r="M5" s="45"/>
+      <c r="O5" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
-      <c r="A5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H5" t="s">
-        <v>33</v>
-      </c>
-      <c r="I5" t="s">
-        <v>34</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="K5" s="38"/>
-      <c r="L5" s="38"/>
-      <c r="M5"/>
-      <c r="N5" t="b">
+    <row r="6" spans="1:15">
+      <c r="A6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" t="s">
+        <v>43</v>
+      </c>
+      <c r="I6" t="s">
+        <v>44</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="K6" s="45" t="s">
+        <v>46</v>
+      </c>
+      <c r="L6" s="45"/>
+      <c r="M6" s="45"/>
+      <c r="N6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:14">
-      <c r="A6" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D6" t="s">
-        <v>37</v>
-      </c>
-      <c r="E6" t="s">
-        <v>19</v>
-      </c>
-      <c r="H6" t="s">
-        <v>38</v>
-      </c>
-      <c r="I6" t="s">
-        <v>39</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="K6" s="38"/>
-      <c r="L6" s="38"/>
-      <c r="M6" t="b">
+      <c r="O6" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="N6" s="1" t="b">
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" t="s">
+        <v>48</v>
+      </c>
+      <c r="I7" t="s">
+        <v>49</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="K7" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="L7" s="45"/>
+      <c r="M7" s="45"/>
+      <c r="N7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:14">
-      <c r="A7" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E7" t="s">
-        <v>19</v>
-      </c>
-      <c r="H7" t="s">
-        <v>42</v>
-      </c>
-      <c r="I7" t="s">
-        <v>43</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="K7" s="38"/>
-      <c r="L7" s="38"/>
-      <c r="M7" t="b">
+      <c r="O7" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="N7" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" ht="13" customHeight="1" spans="1:13">
+    </row>
+    <row r="8" ht="13" customHeight="1" spans="1:14">
       <c r="A8" s="1"/>
       <c r="D8" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="E8" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="H8" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="I8" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="K8" s="38"/>
-      <c r="L8" s="38"/>
-      <c r="M8" t="b">
+        <v>56</v>
+      </c>
+      <c r="K8" s="45" t="s">
+        <v>57</v>
+      </c>
+      <c r="L8" s="45"/>
+      <c r="M8" s="45"/>
+      <c r="N8" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:14">
       <c r="A9" s="1"/>
       <c r="D9" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="E9" t="s">
-        <v>51</v>
-      </c>
-      <c r="F9" s="24" t="s">
-        <v>52</v>
+        <v>59</v>
+      </c>
+      <c r="F9" s="31" t="s">
+        <v>60</v>
       </c>
       <c r="H9" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="I9" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="K9" s="38"/>
-      <c r="L9" s="38"/>
-      <c r="M9" t="b">
+        <v>63</v>
+      </c>
+      <c r="K9" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="L9" s="45"/>
+      <c r="M9" s="45"/>
+      <c r="N9" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:16">
       <c r="A10" s="1"/>
       <c r="D10" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="E10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H10" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="I10" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="K10" s="38"/>
-      <c r="L10" s="38"/>
-      <c r="M10" t="b">
+        <v>68</v>
+      </c>
+      <c r="K10" s="45" t="s">
+        <v>69</v>
+      </c>
+      <c r="L10" s="45"/>
+      <c r="M10" s="45"/>
+      <c r="N10" t="b">
         <v>1</v>
       </c>
-      <c r="O10" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16">
-      <c r="A11" s="26"/>
-      <c r="B11" s="27"/>
-      <c r="C11" s="27"/>
-      <c r="D11" s="28" t="s">
-        <v>61</v>
-      </c>
-      <c r="E11" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="F11" s="32"/>
-      <c r="G11" s="32" t="s">
-        <v>63</v>
-      </c>
-      <c r="H11" s="33" t="s">
-        <v>64</v>
-      </c>
-      <c r="I11" s="33" t="s">
-        <v>65</v>
-      </c>
-      <c r="J11" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="K11" s="39"/>
-      <c r="L11" s="39"/>
-      <c r="M11" s="33" t="b">
+      <c r="P10" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17">
+      <c r="A11" s="32"/>
+      <c r="B11" s="33"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="34" t="s">
+        <v>71</v>
+      </c>
+      <c r="E11" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="F11" s="38"/>
+      <c r="G11" s="38" t="s">
+        <v>73</v>
+      </c>
+      <c r="H11" s="39" t="s">
+        <v>74</v>
+      </c>
+      <c r="I11" s="39" t="s">
+        <v>75</v>
+      </c>
+      <c r="J11" s="46" t="s">
+        <v>76</v>
+      </c>
+      <c r="K11" s="47" t="s">
+        <v>77</v>
+      </c>
+      <c r="L11" s="47"/>
+      <c r="M11" s="47"/>
+      <c r="N11" s="39" t="b">
         <v>1</v>
       </c>
-      <c r="N11" s="33"/>
-      <c r="O11" s="33"/>
-      <c r="P11" s="33"/>
-    </row>
-    <row r="12" spans="1:14">
+      <c r="O11" s="39"/>
+      <c r="P11" s="39"/>
+      <c r="Q11" s="39"/>
+    </row>
+    <row r="12" spans="1:15">
       <c r="A12" s="1" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="D12" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="E12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H12" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="I12" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="K12" s="38"/>
-      <c r="L12" s="38"/>
-      <c r="M12" t="b">
-        <v>1</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="K12" s="45" t="s">
+        <v>83</v>
+      </c>
+      <c r="L12" s="45"/>
+      <c r="M12" s="45"/>
       <c r="N12" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:14">
+      <c r="O12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
       <c r="A13" s="1" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="D13" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
       <c r="E13" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H13" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
       <c r="I13" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="K13" s="38"/>
-      <c r="L13" s="38"/>
-      <c r="M13" t="b">
-        <v>1</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="K13" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="L13" s="45"/>
+      <c r="M13" s="45"/>
       <c r="N13" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:13">
+      <c r="O13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
       <c r="A14" s="1"/>
       <c r="D14" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="E14" t="s">
-        <v>77</v>
-      </c>
-      <c r="F14" s="24" t="s">
-        <v>61</v>
+        <v>90</v>
+      </c>
+      <c r="F14" s="31" t="s">
+        <v>71</v>
       </c>
       <c r="H14" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="I14" t="s">
-        <v>79</v>
+        <v>92</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="K14" s="38"/>
-      <c r="L14" s="38"/>
-      <c r="M14" t="b">
+        <v>93</v>
+      </c>
+      <c r="K14" s="45" t="s">
+        <v>94</v>
+      </c>
+      <c r="L14" s="45"/>
+      <c r="M14" s="45"/>
+      <c r="N14" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:16">
-      <c r="A15" s="26"/>
-      <c r="B15" s="27"/>
-      <c r="C15" s="27"/>
-      <c r="D15" s="28" t="s">
-        <v>61</v>
-      </c>
-      <c r="E15" s="28" t="s">
-        <v>81</v>
-      </c>
-      <c r="F15" s="34"/>
-      <c r="G15" s="34"/>
-      <c r="H15" s="33"/>
-      <c r="I15" s="33"/>
-      <c r="J15" s="40"/>
-      <c r="K15" s="39"/>
-      <c r="L15" s="39"/>
-      <c r="M15" s="33"/>
-      <c r="N15" s="33"/>
-      <c r="O15" s="33"/>
-      <c r="P15" s="33"/>
-    </row>
-    <row r="16" s="21" customFormat="1" spans="1:14">
-      <c r="A16" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="D16" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="E16" s="21" t="s">
-        <v>84</v>
-      </c>
-      <c r="F16" s="35"/>
-      <c r="G16" s="35"/>
-      <c r="H16" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="I16" s="21" t="s">
-        <v>86</v>
+    <row r="15" spans="1:17">
+      <c r="A15" s="32"/>
+      <c r="B15" s="33"/>
+      <c r="C15" s="33"/>
+      <c r="D15" s="34" t="s">
+        <v>71</v>
+      </c>
+      <c r="E15" s="34" t="s">
+        <v>95</v>
+      </c>
+      <c r="F15" s="40"/>
+      <c r="G15" s="40"/>
+      <c r="H15" s="39"/>
+      <c r="I15" s="39"/>
+      <c r="J15" s="39"/>
+      <c r="K15" s="47"/>
+      <c r="L15" s="47"/>
+      <c r="M15" s="47"/>
+      <c r="N15" s="39"/>
+      <c r="O15" s="39"/>
+      <c r="P15" s="39"/>
+      <c r="Q15" s="39"/>
+    </row>
+    <row r="16" s="28" customFormat="1" spans="1:15">
+      <c r="A16" s="35" t="s">
+        <v>96</v>
+      </c>
+      <c r="D16" s="28" t="s">
+        <v>97</v>
+      </c>
+      <c r="E16" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="F16" s="41"/>
+      <c r="G16" s="41"/>
+      <c r="H16" s="28" t="s">
+        <v>99</v>
+      </c>
+      <c r="I16" s="28" t="s">
+        <v>100</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="K16" s="41"/>
-      <c r="L16" s="41"/>
-      <c r="M16" s="21" t="b">
+        <v>101</v>
+      </c>
+      <c r="K16" s="48" t="s">
+        <v>102</v>
+      </c>
+      <c r="L16" s="49"/>
+      <c r="M16" s="49"/>
+      <c r="N16" s="28" t="b">
         <v>1</v>
       </c>
-      <c r="N16" s="21" t="b">
+      <c r="O16" s="28" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="17" s="22" customFormat="1" spans="1:14">
-      <c r="A17" s="30" t="s">
-        <v>82</v>
-      </c>
-      <c r="D17" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="E17" s="22" t="s">
-        <v>89</v>
-      </c>
-      <c r="F17" s="36"/>
-      <c r="G17" s="36"/>
-      <c r="H17" s="22" t="s">
-        <v>90</v>
-      </c>
-      <c r="I17" s="22" t="s">
-        <v>91</v>
+    <row r="17" s="29" customFormat="1" spans="1:15">
+      <c r="A17" s="36" t="s">
+        <v>96</v>
+      </c>
+      <c r="D17" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="E17" s="29" t="s">
+        <v>104</v>
+      </c>
+      <c r="F17" s="42"/>
+      <c r="G17" s="42"/>
+      <c r="H17" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="I17" s="29" t="s">
+        <v>106</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="K17" s="42"/>
-      <c r="L17" s="42"/>
-      <c r="M17" s="22" t="b">
+        <v>107</v>
+      </c>
+      <c r="K17" s="50" t="s">
+        <v>108</v>
+      </c>
+      <c r="L17" s="50"/>
+      <c r="M17" s="50"/>
+      <c r="N17" s="29" t="b">
         <v>1</v>
       </c>
-      <c r="N17" s="22" t="b">
+      <c r="O17" s="29" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="18" s="22" customFormat="1" spans="1:17">
-      <c r="A18" s="30" t="s">
-        <v>82</v>
-      </c>
-      <c r="D18" s="22" t="s">
-        <v>93</v>
-      </c>
-      <c r="E18" s="22" t="s">
-        <v>94</v>
-      </c>
-      <c r="H18" s="22" t="s">
-        <v>95</v>
-      </c>
-      <c r="I18" s="22" t="s">
-        <v>95</v>
+    <row r="18" s="29" customFormat="1" spans="1:18">
+      <c r="A18" s="36" t="s">
+        <v>96</v>
+      </c>
+      <c r="D18" s="29" t="s">
+        <v>109</v>
+      </c>
+      <c r="E18" s="29" t="s">
+        <v>110</v>
+      </c>
+      <c r="H18" s="29" t="s">
+        <v>111</v>
+      </c>
+      <c r="I18" s="29" t="s">
+        <v>111</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="K18" s="42"/>
-      <c r="L18" s="42"/>
-      <c r="N18" s="22" t="b">
+        <v>111</v>
+      </c>
+      <c r="K18" s="50" t="s">
+        <v>112</v>
+      </c>
+      <c r="L18" s="50"/>
+      <c r="M18" s="50"/>
+      <c r="O18" s="29" t="b">
         <v>1</v>
       </c>
-      <c r="Q18" s="22" t="b">
+      <c r="R18" s="29" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="19" s="22" customFormat="1" spans="1:17">
-      <c r="A19" s="30" t="s">
-        <v>82</v>
-      </c>
-      <c r="D19" s="22" t="s">
+    <row r="19" s="29" customFormat="1" spans="1:18">
+      <c r="A19" s="36" t="s">
         <v>96</v>
       </c>
-      <c r="E19" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="H19" s="22" t="s">
-        <v>97</v>
-      </c>
-      <c r="I19" s="22" t="s">
-        <v>97</v>
+      <c r="D19" s="29" t="s">
+        <v>113</v>
+      </c>
+      <c r="E19" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="H19" s="29" t="s">
+        <v>114</v>
+      </c>
+      <c r="I19" s="29" t="s">
+        <v>114</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="K19" s="42"/>
-      <c r="L19" s="42"/>
-      <c r="N19" s="22" t="b">
+        <v>114</v>
+      </c>
+      <c r="K19" s="50" t="s">
+        <v>115</v>
+      </c>
+      <c r="L19" s="50"/>
+      <c r="M19" s="50"/>
+      <c r="O19" s="29" t="b">
         <v>1</v>
       </c>
-      <c r="Q19" s="22" t="b">
+      <c r="R19" s="29" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="20" s="22" customFormat="1" spans="1:17">
-      <c r="A20" s="30" t="s">
-        <v>82</v>
-      </c>
-      <c r="D20" s="22" t="s">
-        <v>98</v>
-      </c>
-      <c r="E20" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="H20" s="22" t="s">
-        <v>99</v>
-      </c>
-      <c r="I20" s="22" t="s">
-        <v>99</v>
+    <row r="20" s="29" customFormat="1" spans="1:18">
+      <c r="A20" s="36" t="s">
+        <v>96</v>
+      </c>
+      <c r="D20" s="29" t="s">
+        <v>116</v>
+      </c>
+      <c r="E20" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="H20" s="29" t="s">
+        <v>117</v>
+      </c>
+      <c r="I20" s="29" t="s">
+        <v>117</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="K20" s="42"/>
-      <c r="L20" s="42"/>
-      <c r="N20" s="22" t="b">
+        <v>117</v>
+      </c>
+      <c r="K20" s="50" t="s">
+        <v>118</v>
+      </c>
+      <c r="L20" s="50"/>
+      <c r="M20" s="50"/>
+      <c r="O20" s="29" t="b">
         <v>1</v>
       </c>
-      <c r="Q20" s="22" t="b">
+      <c r="R20" s="29" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="21" s="23" customFormat="1" spans="1:14">
-      <c r="A21" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="D21" s="23" t="s">
-        <v>100</v>
-      </c>
-      <c r="E21" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="F21" s="37"/>
-      <c r="G21" s="37"/>
-      <c r="H21" s="23" t="s">
-        <v>101</v>
-      </c>
-      <c r="I21" s="23" t="s">
-        <v>102</v>
+    <row r="21" s="30" customFormat="1" spans="1:15">
+      <c r="A21" s="37" t="s">
+        <v>96</v>
+      </c>
+      <c r="D21" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="E21" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="F21" s="43"/>
+      <c r="G21" s="43"/>
+      <c r="H21" s="30" t="s">
+        <v>120</v>
+      </c>
+      <c r="I21" s="30" t="s">
+        <v>121</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="K21" s="43"/>
-      <c r="L21" s="43"/>
-      <c r="M21" s="23" t="b">
+        <v>122</v>
+      </c>
+      <c r="K21" s="51" t="s">
+        <v>123</v>
+      </c>
+      <c r="L21" s="52"/>
+      <c r="M21" s="52"/>
+      <c r="N21" s="30" t="b">
         <v>1</v>
       </c>
-      <c r="N21" s="23" t="b">
+      <c r="O21" s="30" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:13">
       <c r="A22" s="1"/>
-      <c r="K22" s="38"/>
-      <c r="L22" s="38"/>
-    </row>
-    <row r="23" spans="1:12">
+      <c r="K22" s="45"/>
+      <c r="L22" s="45"/>
+      <c r="M22" s="45"/>
+    </row>
+    <row r="23" spans="1:13">
       <c r="A23" s="1"/>
-      <c r="K23" s="38"/>
-      <c r="L23" s="38"/>
-    </row>
-    <row r="24" spans="1:12">
+      <c r="K23" s="45"/>
+      <c r="L23" s="45"/>
+      <c r="M23" s="45"/>
+    </row>
+    <row r="24" spans="1:13">
       <c r="A24" s="1"/>
-      <c r="K24" s="38"/>
-      <c r="L24" s="38"/>
-    </row>
-    <row r="25" spans="1:12">
+      <c r="K24" s="45"/>
+      <c r="L24" s="45"/>
+      <c r="M24" s="45"/>
+    </row>
+    <row r="25" spans="1:13">
       <c r="A25" s="1"/>
-      <c r="K25" s="38"/>
-      <c r="L25" s="38"/>
+      <c r="K25" s="45"/>
+      <c r="L25" s="45"/>
+      <c r="M25" s="45"/>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" s="1"/>
@@ -2517,27 +2724,28 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F47"/>
+  <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.18095238095238" defaultRowHeight="12.75" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9.18095238095238" defaultRowHeight="12.75" outlineLevelCol="6"/>
   <cols>
     <col min="1" max="1" width="12.5428571428571" customWidth="1"/>
     <col min="2" max="2" width="25.8190476190476" style="1" customWidth="1"/>
     <col min="3" max="3" width="35" customWidth="1"/>
     <col min="4" max="5" width="29" customWidth="1"/>
-    <col min="6" max="6" width="13.1809523809524" customWidth="1"/>
+    <col min="6" max="6" width="32.0380952380952" customWidth="1"/>
+    <col min="7" max="7" width="13.1809523809524" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>104</v>
+        <v>124</v>
       </c>
       <c r="C1" t="s">
         <v>7</v>
@@ -2545,375 +2753,441 @@
       <c r="D1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="18" t="s">
         <v>9</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+        <v>10</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>105</v>
+        <v>125</v>
       </c>
       <c r="B2" s="1" t="b">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>106</v>
+        <v>126</v>
       </c>
       <c r="D2" t="s">
-        <v>107</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="1:6">
+        <v>127</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>129</v>
+      </c>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>105</v>
+        <v>125</v>
       </c>
       <c r="B3" s="1" t="b">
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>109</v>
+        <v>130</v>
       </c>
       <c r="D3" t="s">
-        <v>110</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:6">
+        <v>131</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="F3" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="5" t="s">
-        <v>112</v>
+        <v>134</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>113</v>
+        <v>135</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>114</v>
+        <v>136</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="E4" s="18" t="s">
-        <v>116</v>
-      </c>
-      <c r="F4" s="5"/>
-    </row>
-    <row r="5" spans="1:6">
+        <v>137</v>
+      </c>
+      <c r="E4" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="F4" s="22" t="s">
+        <v>139</v>
+      </c>
+      <c r="G4" s="5"/>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="5" t="s">
-        <v>112</v>
+        <v>134</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>117</v>
+        <v>140</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>118</v>
+        <v>141</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="E5" s="18" t="s">
-        <v>120</v>
-      </c>
-      <c r="F5" s="5"/>
-    </row>
-    <row r="6" spans="1:6">
+        <v>142</v>
+      </c>
+      <c r="E5" s="21" t="s">
+        <v>143</v>
+      </c>
+      <c r="F5" s="22" t="s">
+        <v>144</v>
+      </c>
+      <c r="G5" s="5"/>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" s="5" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>121</v>
+        <v>145</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>122</v>
+        <v>146</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="E6" s="18" t="s">
-        <v>124</v>
-      </c>
-      <c r="F6" s="19" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>147</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="F6" s="23" t="s">
+        <v>149</v>
+      </c>
+      <c r="G6" s="24" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="7" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>126</v>
+        <v>151</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>127</v>
+        <v>152</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="E7" s="20" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>153</v>
+      </c>
+      <c r="E7" s="25" t="s">
+        <v>154</v>
+      </c>
+      <c r="F7" s="26" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" s="7" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>130</v>
+        <v>156</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>131</v>
+        <v>157</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="E8" s="20" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+        <v>158</v>
+      </c>
+      <c r="E8" s="25" t="s">
+        <v>159</v>
+      </c>
+      <c r="F8" s="26" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" s="7" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>134</v>
+        <v>161</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>135</v>
+        <v>162</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>136</v>
-      </c>
-      <c r="E9" s="20" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+        <v>163</v>
+      </c>
+      <c r="E9" s="25" t="s">
+        <v>164</v>
+      </c>
+      <c r="F9" s="26" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" s="7" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>138</v>
+        <v>166</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>139</v>
+        <v>167</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="E10" s="20" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+        <v>168</v>
+      </c>
+      <c r="E10" s="25" t="s">
+        <v>169</v>
+      </c>
+      <c r="F10" s="26" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" s="7" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>142</v>
+        <v>171</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>143</v>
+        <v>172</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="E11" s="20" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
+        <v>173</v>
+      </c>
+      <c r="E11" s="25" t="s">
+        <v>174</v>
+      </c>
+      <c r="F11" s="26" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" s="7" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>146</v>
+        <v>176</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>147</v>
+        <v>177</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="E12" s="20" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
+        <v>178</v>
+      </c>
+      <c r="E12" s="25" t="s">
+        <v>179</v>
+      </c>
+      <c r="F12" s="26" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" s="7" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>150</v>
+        <v>181</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>151</v>
+        <v>182</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>152</v>
-      </c>
-      <c r="E13" s="20" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
+        <v>183</v>
+      </c>
+      <c r="E13" s="25" t="s">
+        <v>184</v>
+      </c>
+      <c r="F13" s="26" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" s="7" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>154</v>
+        <v>186</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>155</v>
+        <v>187</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="E14" s="20" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
+        <v>188</v>
+      </c>
+      <c r="E14" s="25" t="s">
+        <v>189</v>
+      </c>
+      <c r="F14" s="26" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>158</v>
+        <v>191</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>159</v>
+        <v>192</v>
       </c>
       <c r="C15" t="s">
-        <v>160</v>
+        <v>193</v>
       </c>
       <c r="D15" t="s">
-        <v>161</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="16" s="4" customFormat="1" spans="1:5">
+        <v>194</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>195</v>
+      </c>
+      <c r="F15" s="26" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="16" s="4" customFormat="1" spans="1:6">
       <c r="A16" s="10" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>163</v>
+        <v>197</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>164</v>
+        <v>198</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="17" s="4" customFormat="1" spans="1:5">
+        <v>199</v>
+      </c>
+      <c r="E16" s="19" t="s">
+        <v>200</v>
+      </c>
+      <c r="F16" s="27" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="17" s="4" customFormat="1" spans="1:6">
       <c r="A17" s="10" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>167</v>
+        <v>202</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>168</v>
+        <v>203</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="18" s="4" customFormat="1" spans="1:5">
+        <v>204</v>
+      </c>
+      <c r="E17" s="19" t="s">
+        <v>205</v>
+      </c>
+      <c r="F17" s="27" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="18" s="4" customFormat="1" spans="1:6">
       <c r="A18" s="10" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>171</v>
+        <v>207</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>172</v>
+        <v>208</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="19" s="4" customFormat="1" spans="1:5">
+        <v>209</v>
+      </c>
+      <c r="E18" s="19" t="s">
+        <v>210</v>
+      </c>
+      <c r="F18" s="27" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="19" s="4" customFormat="1" spans="1:6">
       <c r="A19" s="10" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>175</v>
+        <v>212</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>176</v>
+        <v>213</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="20" s="4" customFormat="1" spans="1:5">
+        <v>214</v>
+      </c>
+      <c r="E19" s="19" t="s">
+        <v>215</v>
+      </c>
+      <c r="F19" s="27" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="20" s="4" customFormat="1" spans="1:6">
       <c r="A20" s="10" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>179</v>
+        <v>217</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>180</v>
+        <v>218</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="21" s="4" customFormat="1" spans="1:5">
+        <v>219</v>
+      </c>
+      <c r="E20" s="19" t="s">
+        <v>220</v>
+      </c>
+      <c r="F20" s="27" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="21" s="4" customFormat="1" spans="1:6">
       <c r="A21" s="10" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>183</v>
+        <v>222</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>184</v>
+        <v>223</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="22" s="4" customFormat="1" spans="1:5">
+        <v>224</v>
+      </c>
+      <c r="E21" s="19" t="s">
+        <v>225</v>
+      </c>
+      <c r="F21" s="27" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="22" s="4" customFormat="1" spans="1:6">
       <c r="A22" s="10" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>187</v>
+        <v>227</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>188</v>
+        <v>228</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>190</v>
+        <v>229</v>
+      </c>
+      <c r="E22" s="19" t="s">
+        <v>230</v>
+      </c>
+      <c r="F22" s="27" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -2921,138 +3195,161 @@
       <c r="B23" s="14"/>
       <c r="C23" s="15"/>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:7">
       <c r="A24" s="13"/>
       <c r="B24" s="14"/>
       <c r="C24" s="16"/>
       <c r="F24" s="15"/>
-    </row>
-    <row r="25" spans="1:6">
+      <c r="G24" s="15"/>
+    </row>
+    <row r="25" spans="1:7">
       <c r="A25" s="13"/>
       <c r="F25" s="15"/>
-    </row>
-    <row r="26" spans="1:6">
+      <c r="G25" s="15"/>
+    </row>
+    <row r="26" spans="1:7">
       <c r="A26" s="7"/>
       <c r="B26" s="17"/>
       <c r="C26" s="9"/>
       <c r="D26" s="9"/>
       <c r="E26" s="9"/>
       <c r="F26" s="15"/>
-    </row>
-    <row r="27" spans="1:6">
+      <c r="G26" s="15"/>
+    </row>
+    <row r="27" spans="1:7">
       <c r="A27" s="7"/>
       <c r="B27" s="17"/>
       <c r="C27" s="9"/>
       <c r="D27" s="9"/>
       <c r="E27" s="9"/>
       <c r="F27" s="16"/>
-    </row>
-    <row r="28" spans="1:6">
+      <c r="G27" s="16"/>
+    </row>
+    <row r="28" spans="1:7">
       <c r="A28" s="7"/>
       <c r="B28" s="17"/>
       <c r="C28" s="9"/>
       <c r="D28" s="9"/>
       <c r="E28" s="9"/>
       <c r="F28" s="15"/>
-    </row>
-    <row r="29" spans="1:6">
+      <c r="G28" s="15"/>
+    </row>
+    <row r="29" spans="1:7">
       <c r="A29" s="7"/>
       <c r="B29" s="17"/>
       <c r="C29" s="9"/>
       <c r="D29" s="9"/>
       <c r="E29" s="9"/>
       <c r="F29" s="15"/>
-    </row>
-    <row r="30" spans="1:6">
+      <c r="G29" s="15"/>
+    </row>
+    <row r="30" spans="1:7">
       <c r="A30" s="7"/>
       <c r="B30" s="17"/>
       <c r="C30" s="9"/>
       <c r="D30" s="9"/>
       <c r="E30" s="9"/>
       <c r="F30" s="15"/>
-    </row>
-    <row r="31" spans="1:6">
+      <c r="G30" s="15"/>
+    </row>
+    <row r="31" spans="1:7">
       <c r="A31" s="13"/>
       <c r="B31" s="14"/>
       <c r="C31" s="15"/>
       <c r="D31" s="15"/>
       <c r="E31" s="15"/>
       <c r="F31" s="16"/>
-    </row>
-    <row r="32" spans="1:6">
+      <c r="G31" s="16"/>
+    </row>
+    <row r="32" spans="1:7">
       <c r="A32" s="13"/>
       <c r="B32" s="14"/>
       <c r="C32" s="15"/>
       <c r="D32" s="15"/>
       <c r="E32" s="15"/>
       <c r="F32" s="15"/>
-    </row>
-    <row r="33" spans="1:6">
+      <c r="G32" s="15"/>
+    </row>
+    <row r="33" spans="1:7">
       <c r="A33" s="13"/>
       <c r="B33" s="14"/>
       <c r="C33" s="15"/>
       <c r="D33" s="15"/>
       <c r="E33" s="15"/>
       <c r="F33" s="15"/>
-    </row>
-    <row r="34" spans="1:6">
+      <c r="G33" s="15"/>
+    </row>
+    <row r="34" spans="1:7">
       <c r="A34" s="13"/>
       <c r="B34" s="14"/>
       <c r="C34" s="15"/>
       <c r="D34" s="15"/>
       <c r="E34" s="15"/>
       <c r="F34" s="15"/>
-    </row>
-    <row r="35" spans="1:6">
+      <c r="G34" s="15"/>
+    </row>
+    <row r="35" spans="1:7">
       <c r="A35" s="13"/>
       <c r="B35" s="14"/>
       <c r="C35" s="15"/>
       <c r="D35" s="15"/>
       <c r="E35" s="15"/>
       <c r="F35" s="15"/>
-    </row>
-    <row r="36" spans="1:6">
+      <c r="G35" s="15"/>
+    </row>
+    <row r="36" spans="1:7">
       <c r="A36" s="13"/>
       <c r="B36" s="14"/>
       <c r="C36" s="15"/>
       <c r="D36" s="15"/>
       <c r="E36" s="15"/>
       <c r="F36" s="15"/>
-    </row>
-    <row r="37" spans="1:6">
+      <c r="G36" s="15"/>
+    </row>
+    <row r="37" spans="1:7">
       <c r="A37" s="13"/>
       <c r="B37" s="14"/>
       <c r="C37" s="15"/>
       <c r="D37" s="15"/>
       <c r="E37" s="15"/>
       <c r="F37" s="15"/>
-    </row>
-    <row r="39" spans="6:6">
+      <c r="G37" s="15"/>
+    </row>
+    <row r="39" spans="6:7">
       <c r="F39" s="15"/>
-    </row>
-    <row r="40" spans="6:6">
+      <c r="G39" s="15"/>
+    </row>
+    <row r="40" spans="6:7">
       <c r="F40" s="15"/>
-    </row>
-    <row r="41" spans="6:6">
+      <c r="G40" s="15"/>
+    </row>
+    <row r="41" spans="6:7">
       <c r="F41" s="15"/>
-    </row>
-    <row r="42" spans="6:6">
+      <c r="G41" s="15"/>
+    </row>
+    <row r="42" spans="6:7">
       <c r="F42" s="16"/>
-    </row>
-    <row r="43" spans="6:6">
+      <c r="G42" s="16"/>
+    </row>
+    <row r="43" spans="6:7">
       <c r="F43" s="15"/>
-    </row>
-    <row r="44" spans="6:6">
+      <c r="G43" s="15"/>
+    </row>
+    <row r="44" spans="6:7">
       <c r="F44" s="15"/>
-    </row>
-    <row r="45" spans="6:6">
+      <c r="G44" s="15"/>
+    </row>
+    <row r="45" spans="6:7">
       <c r="F45" s="15"/>
-    </row>
-    <row r="46" spans="6:6">
+      <c r="G45" s="15"/>
+    </row>
+    <row r="46" spans="6:7">
       <c r="F46" s="15"/>
-    </row>
-    <row r="47" spans="6:6">
+      <c r="G46" s="15"/>
+    </row>
+    <row r="47" spans="6:7">
       <c r="F47" s="15"/>
+      <c r="G47" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3064,66 +3361,74 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.18095238095238" defaultRowHeight="12.75" outlineLevelRow="1" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9.18095238095238" defaultRowHeight="12.75" outlineLevelRow="1" outlineLevelCol="7"/>
   <cols>
     <col min="1" max="1" width="21.7238095238095" customWidth="1"/>
     <col min="2" max="2" width="28.2666666666667" customWidth="1"/>
-    <col min="3" max="4" width="29.7238095238095" customWidth="1"/>
-    <col min="5" max="5" width="12.5428571428571" customWidth="1"/>
-    <col min="6" max="6" width="16.7238095238095" customWidth="1"/>
-    <col min="7" max="7" width="27" customWidth="1"/>
+    <col min="3" max="3" width="29.7238095238095" customWidth="1"/>
+    <col min="4" max="4" width="28.447619047619" customWidth="1"/>
+    <col min="5" max="5" width="25.7142857142857" customWidth="1"/>
+    <col min="6" max="6" width="12.5428571428571" customWidth="1"/>
+    <col min="7" max="7" width="16.7238095238095" customWidth="1"/>
+    <col min="8" max="8" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
-        <v>191</v>
+        <v>232</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>192</v>
+        <v>233</v>
       </c>
       <c r="C1" t="s">
-        <v>193</v>
+        <v>234</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>194</v>
+        <v>235</v>
       </c>
       <c r="E1" t="s">
-        <v>195</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>196</v>
+        <v>236</v>
+      </c>
+      <c r="F1" t="s">
+        <v>237</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+        <v>238</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>198</v>
+        <v>240</v>
       </c>
       <c r="B2" t="s">
-        <v>199</v>
+        <v>241</v>
       </c>
       <c r="C2" t="s">
-        <v>200</v>
+        <v>242</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="E2" s="1">
+        <v>243</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="F2" s="1">
         <v>1</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="G2" s="1" t="s">
-        <v>202</v>
+        <v>71</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>245</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Allow minors to be head of household when there is no adult left in Household   - Affects Death of Heads and ChangeHead of Household   - This helps on situations where the Head died or left the Household - Improve deletion of saved change head of household record - Dont allow to open change head of household if there is only one member in household
</commit_message>
<xml_diff>
--- a/app/src/main/res/raw/change_head_form.xlsx
+++ b/app/src/main/res/raw/change_head_form.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27795" windowHeight="12195" tabRatio="500" activeTab="1"/>
+    <workbookView windowWidth="27645" windowHeight="11970" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="columns" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="251">
   <si>
     <t>group</t>
   </si>
@@ -671,6 +671,21 @@
   </si>
   <si>
     <t xml:space="preserve">የቀድሞው አለቃ ዕድሜ በመብረቅ  </t>
+  </si>
+  <si>
+    <t>HEAD_OUTMIGRATING</t>
+  </si>
+  <si>
+    <t>The Head is Moving out</t>
+  </si>
+  <si>
+    <t>O chefe do agregado está a emigrar</t>
+  </si>
+  <si>
+    <t>Le chef du ménage est en train d’émigrer</t>
+  </si>
+  <si>
+    <t>የቤተሰቡ መሪ እየወጣ ነው</t>
   </si>
   <si>
     <t>DIVORCE</t>
@@ -796,8 +811,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="28">
@@ -847,13 +862,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="0"/>
       <name val="Arial"/>
       <charset val="0"/>
@@ -861,23 +869,21 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -886,6 +892,13 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -901,14 +914,62 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Arial"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -922,59 +983,12 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Arial"/>
@@ -982,10 +996,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Arial"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1039,7 +1054,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1051,7 +1084,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1063,19 +1120,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1087,13 +1168,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1105,7 +1198,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1117,103 +1228,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1291,6 +1306,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1302,33 +1332,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1348,17 +1351,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1374,169 +1371,187 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="34" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="13" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1599,9 +1614,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1648,9 +1660,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="49">
@@ -1979,8 +1989,8 @@
     <col min="3" max="3" width="14.1809523809524" customWidth="1"/>
     <col min="4" max="4" width="20.1809523809524" customWidth="1"/>
     <col min="5" max="5" width="11.7238095238095" customWidth="1"/>
-    <col min="6" max="6" width="12" style="31" customWidth="1"/>
-    <col min="7" max="7" width="20" style="31" customWidth="1"/>
+    <col min="6" max="6" width="12" style="30" customWidth="1"/>
+    <col min="7" max="7" width="20" style="30" customWidth="1"/>
     <col min="8" max="8" width="51.5428571428571" customWidth="1"/>
     <col min="9" max="10" width="55" customWidth="1"/>
     <col min="11" max="11" width="41.6666666666667" customWidth="1"/>
@@ -2006,10 +2016,10 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="31" t="s">
+      <c r="F1" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="31" t="s">
+      <c r="G1" s="30" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -2036,7 +2046,7 @@
       <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="31" t="s">
+      <c r="P1" s="30" t="s">
         <v>15</v>
       </c>
       <c r="Q1" s="1" t="s">
@@ -2067,7 +2077,7 @@
       <c r="J2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="K2" s="44" t="s">
+      <c r="K2" s="43" t="s">
         <v>24</v>
       </c>
       <c r="L2" s="1"/>
@@ -2078,7 +2088,7 @@
       <c r="O2" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="P2" s="31"/>
+      <c r="P2" s="30"/>
     </row>
     <row r="3" spans="1:16">
       <c r="A3" s="1" t="s">
@@ -2101,7 +2111,7 @@
       <c r="J3" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="K3" s="44" t="s">
+      <c r="K3" s="43" t="s">
         <v>29</v>
       </c>
       <c r="L3" s="1"/>
@@ -2112,7 +2122,7 @@
       <c r="O3" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="P3" s="31"/>
+      <c r="P3" s="30"/>
     </row>
     <row r="4" spans="1:15">
       <c r="A4" s="1" t="s">
@@ -2133,11 +2143,11 @@
       <c r="J4" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="K4" s="45" t="s">
+      <c r="K4" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="L4" s="45"/>
-      <c r="M4" s="45"/>
+      <c r="L4" s="44"/>
+      <c r="M4" s="44"/>
       <c r="O4" t="b">
         <v>1</v>
       </c>
@@ -2161,11 +2171,11 @@
       <c r="J5" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="K5" s="45" t="s">
+      <c r="K5" s="44" t="s">
         <v>40</v>
       </c>
-      <c r="L5" s="45"/>
-      <c r="M5" s="45"/>
+      <c r="L5" s="44"/>
+      <c r="M5" s="44"/>
       <c r="O5" t="b">
         <v>1</v>
       </c>
@@ -2189,11 +2199,11 @@
       <c r="J6" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="K6" s="45" t="s">
+      <c r="K6" s="44" t="s">
         <v>46</v>
       </c>
-      <c r="L6" s="45"/>
-      <c r="M6" s="45"/>
+      <c r="L6" s="44"/>
+      <c r="M6" s="44"/>
       <c r="N6" t="b">
         <v>1</v>
       </c>
@@ -2220,11 +2230,11 @@
       <c r="J7" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="K7" s="45" t="s">
+      <c r="K7" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="L7" s="45"/>
-      <c r="M7" s="45"/>
+      <c r="L7" s="44"/>
+      <c r="M7" s="44"/>
       <c r="N7" t="b">
         <v>1</v>
       </c>
@@ -2249,11 +2259,11 @@
       <c r="J8" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="K8" s="45" t="s">
+      <c r="K8" s="44" t="s">
         <v>57</v>
       </c>
-      <c r="L8" s="45"/>
-      <c r="M8" s="45"/>
+      <c r="L8" s="44"/>
+      <c r="M8" s="44"/>
       <c r="N8" t="b">
         <v>1</v>
       </c>
@@ -2266,7 +2276,7 @@
       <c r="E9" t="s">
         <v>59</v>
       </c>
-      <c r="F9" s="31" t="s">
+      <c r="F9" s="30" t="s">
         <v>60</v>
       </c>
       <c r="H9" t="s">
@@ -2278,11 +2288,11 @@
       <c r="J9" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="K9" s="45" t="s">
+      <c r="K9" s="44" t="s">
         <v>64</v>
       </c>
-      <c r="L9" s="45"/>
-      <c r="M9" s="45"/>
+      <c r="L9" s="44"/>
+      <c r="M9" s="44"/>
       <c r="N9" t="b">
         <v>1</v>
       </c>
@@ -2304,11 +2314,11 @@
       <c r="J10" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="K10" s="45" t="s">
+      <c r="K10" s="44" t="s">
         <v>69</v>
       </c>
-      <c r="L10" s="45"/>
-      <c r="M10" s="45"/>
+      <c r="L10" s="44"/>
+      <c r="M10" s="44"/>
       <c r="N10" t="b">
         <v>1</v>
       </c>
@@ -2317,39 +2327,39 @@
       </c>
     </row>
     <row r="11" spans="1:17">
-      <c r="A11" s="32"/>
-      <c r="B11" s="33"/>
-      <c r="C11" s="33"/>
-      <c r="D11" s="34" t="s">
+      <c r="A11" s="31"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="E11" s="34" t="s">
+      <c r="E11" s="33" t="s">
         <v>72</v>
       </c>
-      <c r="F11" s="38"/>
-      <c r="G11" s="38" t="s">
+      <c r="F11" s="37"/>
+      <c r="G11" s="37" t="s">
         <v>73</v>
       </c>
-      <c r="H11" s="39" t="s">
+      <c r="H11" s="38" t="s">
         <v>74</v>
       </c>
-      <c r="I11" s="39" t="s">
+      <c r="I11" s="38" t="s">
         <v>75</v>
       </c>
-      <c r="J11" s="46" t="s">
+      <c r="J11" s="45" t="s">
         <v>76</v>
       </c>
-      <c r="K11" s="47" t="s">
+      <c r="K11" s="46" t="s">
         <v>77</v>
       </c>
-      <c r="L11" s="47"/>
-      <c r="M11" s="47"/>
-      <c r="N11" s="39" t="b">
+      <c r="L11" s="46"/>
+      <c r="M11" s="46"/>
+      <c r="N11" s="38" t="b">
         <v>1</v>
       </c>
-      <c r="O11" s="39"/>
-      <c r="P11" s="39"/>
-      <c r="Q11" s="39"/>
+      <c r="O11" s="38"/>
+      <c r="P11" s="38"/>
+      <c r="Q11" s="38"/>
     </row>
     <row r="12" spans="1:15">
       <c r="A12" s="1" t="s">
@@ -2370,11 +2380,11 @@
       <c r="J12" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="K12" s="45" t="s">
+      <c r="K12" s="44" t="s">
         <v>83</v>
       </c>
-      <c r="L12" s="45"/>
-      <c r="M12" s="45"/>
+      <c r="L12" s="44"/>
+      <c r="M12" s="44"/>
       <c r="N12" t="b">
         <v>1</v>
       </c>
@@ -2401,11 +2411,11 @@
       <c r="J13" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="K13" s="45" t="s">
+      <c r="K13" s="44" t="s">
         <v>88</v>
       </c>
-      <c r="L13" s="45"/>
-      <c r="M13" s="45"/>
+      <c r="L13" s="44"/>
+      <c r="M13" s="44"/>
       <c r="N13" t="b">
         <v>1</v>
       </c>
@@ -2421,7 +2431,7 @@
       <c r="E14" t="s">
         <v>90</v>
       </c>
-      <c r="F14" s="31" t="s">
+      <c r="F14" s="30" t="s">
         <v>71</v>
       </c>
       <c r="H14" t="s">
@@ -2433,253 +2443,253 @@
       <c r="J14" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="K14" s="45" t="s">
+      <c r="K14" s="44" t="s">
         <v>94</v>
       </c>
-      <c r="L14" s="45"/>
-      <c r="M14" s="45"/>
+      <c r="L14" s="44"/>
+      <c r="M14" s="44"/>
       <c r="N14" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:17">
-      <c r="A15" s="32"/>
-      <c r="B15" s="33"/>
-      <c r="C15" s="33"/>
-      <c r="D15" s="34" t="s">
+      <c r="A15" s="31"/>
+      <c r="B15" s="32"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="E15" s="34" t="s">
+      <c r="E15" s="33" t="s">
         <v>95</v>
       </c>
-      <c r="F15" s="40"/>
-      <c r="G15" s="40"/>
-      <c r="H15" s="39"/>
-      <c r="I15" s="39"/>
-      <c r="J15" s="39"/>
-      <c r="K15" s="47"/>
-      <c r="L15" s="47"/>
-      <c r="M15" s="47"/>
-      <c r="N15" s="39"/>
-      <c r="O15" s="39"/>
-      <c r="P15" s="39"/>
-      <c r="Q15" s="39"/>
-    </row>
-    <row r="16" s="28" customFormat="1" spans="1:15">
-      <c r="A16" s="35" t="s">
+      <c r="F15" s="39"/>
+      <c r="G15" s="39"/>
+      <c r="H15" s="38"/>
+      <c r="I15" s="38"/>
+      <c r="J15" s="38"/>
+      <c r="K15" s="46"/>
+      <c r="L15" s="46"/>
+      <c r="M15" s="46"/>
+      <c r="N15" s="38"/>
+      <c r="O15" s="38"/>
+      <c r="P15" s="38"/>
+      <c r="Q15" s="38"/>
+    </row>
+    <row r="16" s="27" customFormat="1" spans="1:15">
+      <c r="A16" s="34" t="s">
         <v>96</v>
       </c>
-      <c r="D16" s="28" t="s">
+      <c r="D16" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="E16" s="28" t="s">
+      <c r="E16" s="27" t="s">
         <v>98</v>
       </c>
-      <c r="F16" s="41"/>
-      <c r="G16" s="41"/>
-      <c r="H16" s="28" t="s">
+      <c r="F16" s="40"/>
+      <c r="G16" s="40"/>
+      <c r="H16" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="I16" s="28" t="s">
+      <c r="I16" s="27" t="s">
         <v>100</v>
       </c>
       <c r="J16" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="K16" s="48" t="s">
+      <c r="K16" s="47" t="s">
         <v>102</v>
       </c>
-      <c r="L16" s="49"/>
-      <c r="M16" s="49"/>
-      <c r="N16" s="28" t="b">
+      <c r="L16" s="47"/>
+      <c r="M16" s="47"/>
+      <c r="N16" s="27" t="b">
         <v>1</v>
       </c>
-      <c r="O16" s="28" t="b">
+      <c r="O16" s="27" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="17" s="29" customFormat="1" spans="1:15">
-      <c r="A17" s="36" t="s">
+    <row r="17" s="28" customFormat="1" spans="1:15">
+      <c r="A17" s="35" t="s">
         <v>96</v>
       </c>
-      <c r="D17" s="29" t="s">
+      <c r="D17" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="E17" s="29" t="s">
+      <c r="E17" s="28" t="s">
         <v>104</v>
       </c>
-      <c r="F17" s="42"/>
-      <c r="G17" s="42"/>
-      <c r="H17" s="29" t="s">
+      <c r="F17" s="41"/>
+      <c r="G17" s="41"/>
+      <c r="H17" s="28" t="s">
         <v>105</v>
       </c>
-      <c r="I17" s="29" t="s">
+      <c r="I17" s="28" t="s">
         <v>106</v>
       </c>
       <c r="J17" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="K17" s="50" t="s">
+      <c r="K17" s="48" t="s">
         <v>108</v>
       </c>
-      <c r="L17" s="50"/>
-      <c r="M17" s="50"/>
-      <c r="N17" s="29" t="b">
+      <c r="L17" s="48"/>
+      <c r="M17" s="48"/>
+      <c r="N17" s="28" t="b">
         <v>1</v>
       </c>
-      <c r="O17" s="29" t="b">
+      <c r="O17" s="28" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="18" s="29" customFormat="1" spans="1:18">
-      <c r="A18" s="36" t="s">
+    <row r="18" s="28" customFormat="1" spans="1:18">
+      <c r="A18" s="35" t="s">
         <v>96</v>
       </c>
-      <c r="D18" s="29" t="s">
+      <c r="D18" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="E18" s="29" t="s">
+      <c r="E18" s="28" t="s">
         <v>110</v>
       </c>
-      <c r="H18" s="29" t="s">
+      <c r="H18" s="28" t="s">
         <v>111</v>
       </c>
-      <c r="I18" s="29" t="s">
+      <c r="I18" s="28" t="s">
         <v>111</v>
       </c>
       <c r="J18" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="K18" s="50" t="s">
+      <c r="K18" s="48" t="s">
         <v>112</v>
       </c>
-      <c r="L18" s="50"/>
-      <c r="M18" s="50"/>
-      <c r="O18" s="29" t="b">
+      <c r="L18" s="48"/>
+      <c r="M18" s="48"/>
+      <c r="O18" s="28" t="b">
         <v>1</v>
       </c>
-      <c r="R18" s="29" t="b">
+      <c r="R18" s="28" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="19" s="29" customFormat="1" spans="1:18">
-      <c r="A19" s="36" t="s">
+    <row r="19" s="28" customFormat="1" spans="1:18">
+      <c r="A19" s="35" t="s">
         <v>96</v>
       </c>
-      <c r="D19" s="29" t="s">
+      <c r="D19" s="28" t="s">
         <v>113</v>
       </c>
-      <c r="E19" s="29" t="s">
+      <c r="E19" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="H19" s="29" t="s">
+      <c r="H19" s="28" t="s">
         <v>114</v>
       </c>
-      <c r="I19" s="29" t="s">
+      <c r="I19" s="28" t="s">
         <v>114</v>
       </c>
       <c r="J19" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="K19" s="50" t="s">
+      <c r="K19" s="48" t="s">
         <v>115</v>
       </c>
-      <c r="L19" s="50"/>
-      <c r="M19" s="50"/>
-      <c r="O19" s="29" t="b">
+      <c r="L19" s="48"/>
+      <c r="M19" s="48"/>
+      <c r="O19" s="28" t="b">
         <v>1</v>
       </c>
-      <c r="R19" s="29" t="b">
+      <c r="R19" s="28" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="20" s="29" customFormat="1" spans="1:18">
-      <c r="A20" s="36" t="s">
+    <row r="20" s="28" customFormat="1" spans="1:18">
+      <c r="A20" s="35" t="s">
         <v>96</v>
       </c>
-      <c r="D20" s="29" t="s">
+      <c r="D20" s="28" t="s">
         <v>116</v>
       </c>
-      <c r="E20" s="29" t="s">
+      <c r="E20" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="H20" s="29" t="s">
+      <c r="H20" s="28" t="s">
         <v>117</v>
       </c>
-      <c r="I20" s="29" t="s">
+      <c r="I20" s="28" t="s">
         <v>117</v>
       </c>
       <c r="J20" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="K20" s="50" t="s">
+      <c r="K20" s="48" t="s">
         <v>118</v>
       </c>
-      <c r="L20" s="50"/>
-      <c r="M20" s="50"/>
-      <c r="O20" s="29" t="b">
+      <c r="L20" s="48"/>
+      <c r="M20" s="48"/>
+      <c r="O20" s="28" t="b">
         <v>1</v>
       </c>
-      <c r="R20" s="29" t="b">
+      <c r="R20" s="28" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="21" s="30" customFormat="1" spans="1:15">
-      <c r="A21" s="37" t="s">
+    <row r="21" s="29" customFormat="1" spans="1:15">
+      <c r="A21" s="36" t="s">
         <v>96</v>
       </c>
-      <c r="D21" s="30" t="s">
+      <c r="D21" s="29" t="s">
         <v>119</v>
       </c>
-      <c r="E21" s="30" t="s">
+      <c r="E21" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="F21" s="43"/>
-      <c r="G21" s="43"/>
-      <c r="H21" s="30" t="s">
+      <c r="F21" s="42"/>
+      <c r="G21" s="42"/>
+      <c r="H21" s="29" t="s">
         <v>120</v>
       </c>
-      <c r="I21" s="30" t="s">
+      <c r="I21" s="29" t="s">
         <v>121</v>
       </c>
       <c r="J21" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="K21" s="51" t="s">
+      <c r="K21" s="49" t="s">
         <v>123</v>
       </c>
-      <c r="L21" s="52"/>
-      <c r="M21" s="52"/>
-      <c r="N21" s="30" t="b">
+      <c r="L21" s="49"/>
+      <c r="M21" s="49"/>
+      <c r="N21" s="29" t="b">
         <v>1</v>
       </c>
-      <c r="O21" s="30" t="b">
+      <c r="O21" s="29" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:13">
       <c r="A22" s="1"/>
-      <c r="K22" s="45"/>
-      <c r="L22" s="45"/>
-      <c r="M22" s="45"/>
+      <c r="K22" s="44"/>
+      <c r="L22" s="44"/>
+      <c r="M22" s="44"/>
     </row>
     <row r="23" spans="1:13">
       <c r="A23" s="1"/>
-      <c r="K23" s="45"/>
-      <c r="L23" s="45"/>
-      <c r="M23" s="45"/>
+      <c r="K23" s="44"/>
+      <c r="L23" s="44"/>
+      <c r="M23" s="44"/>
     </row>
     <row r="24" spans="1:13">
       <c r="A24" s="1"/>
-      <c r="K24" s="45"/>
-      <c r="L24" s="45"/>
-      <c r="M24" s="45"/>
+      <c r="K24" s="44"/>
+      <c r="L24" s="44"/>
+      <c r="M24" s="44"/>
     </row>
     <row r="25" spans="1:13">
       <c r="A25" s="1"/>
-      <c r="K25" s="45"/>
-      <c r="L25" s="45"/>
-      <c r="M25" s="45"/>
+      <c r="K25" s="44"/>
+      <c r="L25" s="44"/>
+      <c r="M25" s="44"/>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" s="1"/>
@@ -2724,10 +2734,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G47"/>
+  <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F22"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A17" sqref="$A17:$XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.18095238095238" defaultRowHeight="12.75" outlineLevelCol="6"/>
@@ -2886,7 +2896,7 @@
       <c r="E7" s="25" t="s">
         <v>154</v>
       </c>
-      <c r="F7" s="26" t="s">
+      <c r="F7" s="20" t="s">
         <v>155</v>
       </c>
     </row>
@@ -2906,7 +2916,7 @@
       <c r="E8" s="25" t="s">
         <v>159</v>
       </c>
-      <c r="F8" s="26" t="s">
+      <c r="F8" s="20" t="s">
         <v>160</v>
       </c>
     </row>
@@ -2926,7 +2936,7 @@
       <c r="E9" s="25" t="s">
         <v>164</v>
       </c>
-      <c r="F9" s="26" t="s">
+      <c r="F9" s="20" t="s">
         <v>165</v>
       </c>
     </row>
@@ -2946,7 +2956,7 @@
       <c r="E10" s="25" t="s">
         <v>169</v>
       </c>
-      <c r="F10" s="26" t="s">
+      <c r="F10" s="20" t="s">
         <v>170</v>
       </c>
     </row>
@@ -2966,7 +2976,7 @@
       <c r="E11" s="25" t="s">
         <v>174</v>
       </c>
-      <c r="F11" s="26" t="s">
+      <c r="F11" s="20" t="s">
         <v>175</v>
       </c>
     </row>
@@ -2986,7 +2996,7 @@
       <c r="E12" s="25" t="s">
         <v>179</v>
       </c>
-      <c r="F12" s="26" t="s">
+      <c r="F12" s="20" t="s">
         <v>180</v>
       </c>
     </row>
@@ -3006,7 +3016,7 @@
       <c r="E13" s="25" t="s">
         <v>184</v>
       </c>
-      <c r="F13" s="26" t="s">
+      <c r="F13" s="20" t="s">
         <v>185</v>
       </c>
     </row>
@@ -3026,7 +3036,7 @@
       <c r="E14" s="25" t="s">
         <v>189</v>
       </c>
-      <c r="F14" s="26" t="s">
+      <c r="F14" s="20" t="s">
         <v>190</v>
       </c>
     </row>
@@ -3046,7 +3056,7 @@
       <c r="E15" s="19" t="s">
         <v>195</v>
       </c>
-      <c r="F15" s="26" t="s">
+      <c r="F15" s="20" t="s">
         <v>196</v>
       </c>
     </row>
@@ -3066,7 +3076,7 @@
       <c r="E16" s="19" t="s">
         <v>200</v>
       </c>
-      <c r="F16" s="27" t="s">
+      <c r="F16" s="26" t="s">
         <v>201</v>
       </c>
     </row>
@@ -3086,7 +3096,7 @@
       <c r="E17" s="19" t="s">
         <v>205</v>
       </c>
-      <c r="F17" s="27" t="s">
+      <c r="F17" s="26" t="s">
         <v>206</v>
       </c>
     </row>
@@ -3106,7 +3116,7 @@
       <c r="E18" s="19" t="s">
         <v>210</v>
       </c>
-      <c r="F18" s="27" t="s">
+      <c r="F18" s="26" t="s">
         <v>211</v>
       </c>
     </row>
@@ -3126,7 +3136,7 @@
       <c r="E19" s="19" t="s">
         <v>215</v>
       </c>
-      <c r="F19" s="27" t="s">
+      <c r="F19" s="26" t="s">
         <v>216</v>
       </c>
     </row>
@@ -3146,7 +3156,7 @@
       <c r="E20" s="19" t="s">
         <v>220</v>
       </c>
-      <c r="F20" s="27" t="s">
+      <c r="F20" s="26" t="s">
         <v>221</v>
       </c>
     </row>
@@ -3166,7 +3176,7 @@
       <c r="E21" s="19" t="s">
         <v>225</v>
       </c>
-      <c r="F21" s="27" t="s">
+      <c r="F21" s="26" t="s">
         <v>226</v>
       </c>
     </row>
@@ -3186,33 +3196,44 @@
       <c r="E22" s="19" t="s">
         <v>230</v>
       </c>
-      <c r="F22" s="27" t="s">
+      <c r="F22" s="26" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="13"/>
-      <c r="B23" s="14"/>
-      <c r="C23" s="15"/>
-    </row>
-    <row r="24" spans="1:7">
+    <row r="23" s="4" customFormat="1" spans="1:6">
+      <c r="A23" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>233</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="E23" s="19" t="s">
+        <v>235</v>
+      </c>
+      <c r="F23" s="26" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
       <c r="A24" s="13"/>
       <c r="B24" s="14"/>
-      <c r="C24" s="16"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="15"/>
+      <c r="C24" s="15"/>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="13"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="16"/>
       <c r="F25" s="15"/>
       <c r="G25" s="15"/>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="7"/>
-      <c r="B26" s="17"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="9"/>
-      <c r="E26" s="9"/>
+      <c r="A26" s="13"/>
       <c r="F26" s="15"/>
       <c r="G26" s="15"/>
     </row>
@@ -3222,8 +3243,8 @@
       <c r="C27" s="9"/>
       <c r="D27" s="9"/>
       <c r="E27" s="9"/>
-      <c r="F27" s="16"/>
-      <c r="G27" s="16"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="15"/>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="7"/>
@@ -3231,8 +3252,8 @@
       <c r="C28" s="9"/>
       <c r="D28" s="9"/>
       <c r="E28" s="9"/>
-      <c r="F28" s="15"/>
-      <c r="G28" s="15"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="16"/>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="7"/>
@@ -3253,13 +3274,13 @@
       <c r="G30" s="15"/>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" s="13"/>
-      <c r="B31" s="14"/>
-      <c r="C31" s="15"/>
-      <c r="D31" s="15"/>
-      <c r="E31" s="15"/>
-      <c r="F31" s="16"/>
-      <c r="G31" s="16"/>
+      <c r="A31" s="7"/>
+      <c r="B31" s="17"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="15"/>
+      <c r="G31" s="15"/>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="13"/>
@@ -3267,8 +3288,8 @@
       <c r="C32" s="15"/>
       <c r="D32" s="15"/>
       <c r="E32" s="15"/>
-      <c r="F32" s="15"/>
-      <c r="G32" s="15"/>
+      <c r="F32" s="16"/>
+      <c r="G32" s="16"/>
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="13"/>
@@ -3315,9 +3336,14 @@
       <c r="F37" s="15"/>
       <c r="G37" s="15"/>
     </row>
-    <row r="39" spans="6:7">
-      <c r="F39" s="15"/>
-      <c r="G39" s="15"/>
+    <row r="38" spans="1:7">
+      <c r="A38" s="13"/>
+      <c r="B38" s="14"/>
+      <c r="C38" s="15"/>
+      <c r="D38" s="15"/>
+      <c r="E38" s="15"/>
+      <c r="F38" s="15"/>
+      <c r="G38" s="15"/>
     </row>
     <row r="40" spans="6:7">
       <c r="F40" s="15"/>
@@ -3328,12 +3354,12 @@
       <c r="G41" s="15"/>
     </row>
     <row r="42" spans="6:7">
-      <c r="F42" s="16"/>
-      <c r="G42" s="16"/>
+      <c r="F42" s="15"/>
+      <c r="G42" s="15"/>
     </row>
     <row r="43" spans="6:7">
-      <c r="F43" s="15"/>
-      <c r="G43" s="15"/>
+      <c r="F43" s="16"/>
+      <c r="G43" s="16"/>
     </row>
     <row r="44" spans="6:7">
       <c r="F44" s="15"/>
@@ -3350,6 +3376,10 @@
     <row r="47" spans="6:7">
       <c r="F47" s="15"/>
       <c r="G47" s="15"/>
+    </row>
+    <row r="48" spans="6:7">
+      <c r="F48" s="15"/>
+      <c r="G48" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3381,45 +3411,45 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
-        <v>232</v>
+        <v>237</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="C1" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="E1" t="s">
-        <v>236</v>
+        <v>241</v>
       </c>
       <c r="F1" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>240</v>
+        <v>245</v>
       </c>
       <c r="B2" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C2" t="s">
-        <v>242</v>
+        <v>247</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>243</v>
+        <v>248</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="F2" s="1">
         <v>1</v>
@@ -3428,7 +3458,7 @@
         <v>71</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>245</v>
+        <v>250</v>
       </c>
     </row>
   </sheetData>

</xml_diff>